<commit_message>
One not yet complete file update.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/Prelim2025/DoD_2025_Prelim.xlsx
+++ b/Output/AcqTrends/Prelim2025/DoD_2025_Prelim.xlsx
@@ -244,8 +244,8 @@
     <numFmt numFmtId="184" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="189" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="185" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="190" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="191" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="192" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -291,8 +291,8 @@
     <xf numFmtId="184" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="189" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="185" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="190" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="191" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="192" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3213,92 +3213,92 @@
       <c r="N2" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5" t="n">
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10" t="n">
         <v>59180597697.378</v>
       </c>
-      <c r="Z2" s="5" t="n">
+      <c r="Z2" s="10" t="n">
         <v>68029133140.4963</v>
       </c>
-      <c r="AA2" s="5" t="n">
+      <c r="AA2" s="10" t="n">
         <v>84172927045.2604</v>
       </c>
-      <c r="AB2" s="5" t="n">
+      <c r="AB2" s="10" t="n">
         <v>109191257117.131</v>
       </c>
-      <c r="AC2" s="5" t="n">
+      <c r="AC2" s="10" t="n">
         <v>109916829388.952</v>
       </c>
-      <c r="AD2" s="5" t="n">
+      <c r="AD2" s="10" t="n">
         <v>128055920615.379</v>
       </c>
-      <c r="AE2" s="5" t="n">
+      <c r="AE2" s="10" t="n">
         <v>145646321248.104</v>
       </c>
-      <c r="AF2" s="5" t="n">
+      <c r="AF2" s="10" t="n">
         <v>166847504445.292</v>
       </c>
-      <c r="AG2" s="5" t="n">
+      <c r="AG2" s="10" t="n">
         <v>193683604329.733</v>
       </c>
-      <c r="AH2" s="5" t="n">
+      <c r="AH2" s="10" t="n">
         <v>174919592258.472</v>
       </c>
-      <c r="AI2" s="5" t="n">
+      <c r="AI2" s="10" t="n">
         <v>190999962236.724</v>
       </c>
-      <c r="AJ2" s="5" t="n">
+      <c r="AJ2" s="10" t="n">
         <v>185453438471.699</v>
       </c>
-      <c r="AK2" s="5" t="n">
+      <c r="AK2" s="10" t="n">
         <v>172452411014.604</v>
       </c>
-      <c r="AL2" s="5" t="n">
+      <c r="AL2" s="10" t="n">
         <v>146688840548.586</v>
       </c>
-      <c r="AM2" s="5" t="n">
+      <c r="AM2" s="10" t="n">
         <v>145768921953.585</v>
       </c>
-      <c r="AN2" s="5" t="n">
+      <c r="AN2" s="10" t="n">
         <v>141434777332.903</v>
       </c>
-      <c r="AO2" s="5" t="n">
+      <c r="AO2" s="10" t="n">
         <v>151076383014.59</v>
       </c>
-      <c r="AP2" s="5" t="n">
+      <c r="AP2" s="10" t="n">
         <v>156657509545.924</v>
       </c>
-      <c r="AQ2" s="5" t="n">
+      <c r="AQ2" s="10" t="n">
         <v>179109699516.117</v>
       </c>
-      <c r="AR2" s="5" t="n">
+      <c r="AR2" s="10" t="n">
         <v>193460168755.637</v>
       </c>
-      <c r="AS2" s="5" t="n">
+      <c r="AS2" s="10" t="n">
         <v>214818853679.889</v>
       </c>
-      <c r="AT2" s="5" t="n">
+      <c r="AT2" s="10" t="n">
         <v>212566660802.25</v>
       </c>
-      <c r="AU2" s="5" t="n">
+      <c r="AU2" s="10" t="n">
         <v>221282124184.548</v>
       </c>
-      <c r="AV2" s="5" t="n">
+      <c r="AV2" s="10" t="n">
         <v>229155776069.99</v>
       </c>
-      <c r="AW2" s="5" t="n">
+      <c r="AW2" s="10" t="n">
         <v>223337217801.76</v>
       </c>
-      <c r="AX2" s="5"/>
+      <c r="AX2" s="10"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -3313,92 +3313,92 @@
       <c r="N3" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5" t="n">
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10" t="n">
         <v>5866981783</v>
       </c>
-      <c r="Z3" s="5" t="n">
+      <c r="Z3" s="10" t="n">
         <v>8355043007</v>
       </c>
-      <c r="AA3" s="5" t="n">
+      <c r="AA3" s="10" t="n">
         <v>8568508430</v>
       </c>
-      <c r="AB3" s="5" t="n">
+      <c r="AB3" s="10" t="n">
         <v>9446210344.1396</v>
       </c>
-      <c r="AC3" s="5" t="n">
+      <c r="AC3" s="10" t="n">
         <v>11392034495.2552</v>
       </c>
-      <c r="AD3" s="5" t="n">
+      <c r="AD3" s="10" t="n">
         <v>22074131513.6508</v>
       </c>
-      <c r="AE3" s="5" t="n">
+      <c r="AE3" s="10" t="n">
         <v>19496741799.8163</v>
       </c>
-      <c r="AF3" s="5" t="n">
+      <c r="AF3" s="10" t="n">
         <v>17332396700.2473</v>
       </c>
-      <c r="AG3" s="5" t="n">
+      <c r="AG3" s="10" t="n">
         <v>22695323709.5189</v>
       </c>
-      <c r="AH3" s="5" t="n">
+      <c r="AH3" s="10" t="n">
         <v>24305277577.0872</v>
       </c>
-      <c r="AI3" s="5" t="n">
+      <c r="AI3" s="10" t="n">
         <v>17166981775.4083</v>
       </c>
-      <c r="AJ3" s="5" t="n">
+      <c r="AJ3" s="10" t="n">
         <v>19616137972.3993</v>
       </c>
-      <c r="AK3" s="5" t="n">
+      <c r="AK3" s="10" t="n">
         <v>27116363534.6684</v>
       </c>
-      <c r="AL3" s="5" t="n">
+      <c r="AL3" s="10" t="n">
         <v>18305960685.1594</v>
       </c>
-      <c r="AM3" s="5" t="n">
+      <c r="AM3" s="10" t="n">
         <v>11857612390.5243</v>
       </c>
-      <c r="AN3" s="5" t="n">
+      <c r="AN3" s="10" t="n">
         <v>8979268726.5904</v>
       </c>
-      <c r="AO3" s="5" t="n">
+      <c r="AO3" s="10" t="n">
         <v>7378144851.9658</v>
       </c>
-      <c r="AP3" s="5" t="n">
+      <c r="AP3" s="10" t="n">
         <v>9206054541.7008</v>
       </c>
-      <c r="AQ3" s="5" t="n">
+      <c r="AQ3" s="10" t="n">
         <v>10484521166.6575</v>
       </c>
-      <c r="AR3" s="5" t="n">
+      <c r="AR3" s="10" t="n">
         <v>9749228354.0059</v>
       </c>
-      <c r="AS3" s="5" t="n">
+      <c r="AS3" s="10" t="n">
         <v>8878683422.4911</v>
       </c>
-      <c r="AT3" s="5" t="n">
+      <c r="AT3" s="10" t="n">
         <v>10360675618.2093</v>
       </c>
-      <c r="AU3" s="5" t="n">
+      <c r="AU3" s="10" t="n">
         <v>17515768686.6156</v>
       </c>
-      <c r="AV3" s="5" t="n">
+      <c r="AV3" s="10" t="n">
         <v>16776830306.481</v>
       </c>
-      <c r="AW3" s="5" t="n">
+      <c r="AW3" s="10" t="n">
         <v>17419499858.04</v>
       </c>
-      <c r="AX3" s="5"/>
+      <c r="AX3" s="10"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -3413,92 +3413,92 @@
       <c r="N4" t="s">
         <v>57</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5" t="n">
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10" t="n">
         <v>972819279</v>
       </c>
-      <c r="Z4" s="5" t="n">
+      <c r="Z4" s="10" t="n">
         <v>1570724370.5388</v>
       </c>
-      <c r="AA4" s="5" t="n">
+      <c r="AA4" s="10" t="n">
         <v>1753774695.64</v>
       </c>
-      <c r="AB4" s="5" t="n">
+      <c r="AB4" s="10" t="n">
         <v>2126173998.58</v>
       </c>
-      <c r="AC4" s="5" t="n">
+      <c r="AC4" s="10" t="n">
         <v>2422119314.4787</v>
       </c>
-      <c r="AD4" s="5" t="n">
+      <c r="AD4" s="10" t="n">
         <v>2494335831.8172</v>
       </c>
-      <c r="AE4" s="5" t="n">
+      <c r="AE4" s="10" t="n">
         <v>2359548085.2906</v>
       </c>
-      <c r="AF4" s="5" t="n">
+      <c r="AF4" s="10" t="n">
         <v>1688436144.1354</v>
       </c>
-      <c r="AG4" s="5" t="n">
+      <c r="AG4" s="10" t="n">
         <v>2704344656.9408</v>
       </c>
-      <c r="AH4" s="5" t="n">
+      <c r="AH4" s="10" t="n">
         <v>1809665944.0899</v>
       </c>
-      <c r="AI4" s="5" t="n">
+      <c r="AI4" s="10" t="n">
         <v>1829730576.1443</v>
       </c>
-      <c r="AJ4" s="5" t="n">
+      <c r="AJ4" s="10" t="n">
         <v>1938581347.4045</v>
       </c>
-      <c r="AK4" s="5" t="n">
+      <c r="AK4" s="10" t="n">
         <v>1220801966.4954</v>
       </c>
-      <c r="AL4" s="5" t="n">
+      <c r="AL4" s="10" t="n">
         <v>654738316.8306</v>
       </c>
-      <c r="AM4" s="5" t="n">
+      <c r="AM4" s="10" t="n">
         <v>472312874.5174</v>
       </c>
-      <c r="AN4" s="5" t="n">
+      <c r="AN4" s="10" t="n">
         <v>541724638.1255</v>
       </c>
-      <c r="AO4" s="5" t="n">
+      <c r="AO4" s="10" t="n">
         <v>555617181.8077</v>
       </c>
-      <c r="AP4" s="5" t="n">
+      <c r="AP4" s="10" t="n">
         <v>490378558.3192</v>
       </c>
-      <c r="AQ4" s="5" t="n">
+      <c r="AQ4" s="10" t="n">
         <v>440263526.8345</v>
       </c>
-      <c r="AR4" s="5" t="n">
+      <c r="AR4" s="10" t="n">
         <v>784505779.7384</v>
       </c>
-      <c r="AS4" s="5" t="n">
+      <c r="AS4" s="10" t="n">
         <v>1120331895.2647</v>
       </c>
-      <c r="AT4" s="5" t="n">
+      <c r="AT4" s="10" t="n">
         <v>1217674990.7416</v>
       </c>
-      <c r="AU4" s="5" t="n">
+      <c r="AU4" s="10" t="n">
         <v>1045016396.2211</v>
       </c>
-      <c r="AV4" s="5" t="n">
+      <c r="AV4" s="10" t="n">
         <v>1231672307.5974</v>
       </c>
-      <c r="AW4" s="5" t="n">
+      <c r="AW4" s="10" t="n">
         <v>1674889726.57</v>
       </c>
-      <c r="AX4" s="5"/>
+      <c r="AX4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -3513,92 +3513,92 @@
       <c r="N5" t="s">
         <v>59</v>
       </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5" t="n">
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10" t="n">
         <v>3291545650</v>
       </c>
-      <c r="Z5" s="5" t="n">
+      <c r="Z5" s="10" t="n">
         <v>3143486709</v>
       </c>
-      <c r="AA5" s="5" t="n">
+      <c r="AA5" s="10" t="n">
         <v>3345169156</v>
       </c>
-      <c r="AB5" s="5" t="n">
+      <c r="AB5" s="10" t="n">
         <v>5351937141.05</v>
       </c>
-      <c r="AC5" s="5" t="n">
+      <c r="AC5" s="10" t="n">
         <v>6684892601.61</v>
       </c>
-      <c r="AD5" s="5" t="n">
+      <c r="AD5" s="10" t="n">
         <v>10414113301.3569</v>
       </c>
-      <c r="AE5" s="5" t="n">
+      <c r="AE5" s="10" t="n">
         <v>13722589382.0111</v>
       </c>
-      <c r="AF5" s="5" t="n">
+      <c r="AF5" s="10" t="n">
         <v>13968024141.3283</v>
       </c>
-      <c r="AG5" s="5" t="n">
+      <c r="AG5" s="10" t="n">
         <v>18056879490.7396</v>
       </c>
-      <c r="AH5" s="5" t="n">
+      <c r="AH5" s="10" t="n">
         <v>14820879349.2833</v>
       </c>
-      <c r="AI5" s="5" t="n">
+      <c r="AI5" s="10" t="n">
         <v>19828399352.6762</v>
       </c>
-      <c r="AJ5" s="5" t="n">
+      <c r="AJ5" s="10" t="n">
         <v>26969280878.0824</v>
       </c>
-      <c r="AK5" s="5" t="n">
+      <c r="AK5" s="10" t="n">
         <v>18077028467.1119</v>
       </c>
-      <c r="AL5" s="5" t="n">
+      <c r="AL5" s="10" t="n">
         <v>17615332077.3368</v>
       </c>
-      <c r="AM5" s="5" t="n">
+      <c r="AM5" s="10" t="n">
         <v>14461482018.4858</v>
       </c>
-      <c r="AN5" s="5" t="n">
+      <c r="AN5" s="10" t="n">
         <v>12601321121.1564</v>
       </c>
-      <c r="AO5" s="5" t="n">
+      <c r="AO5" s="10" t="n">
         <v>13209086097.471</v>
       </c>
-      <c r="AP5" s="5" t="n">
+      <c r="AP5" s="10" t="n">
         <v>16602157338.5228</v>
       </c>
-      <c r="AQ5" s="5" t="n">
+      <c r="AQ5" s="10" t="n">
         <v>15728961093.0458</v>
       </c>
-      <c r="AR5" s="5" t="n">
+      <c r="AR5" s="10" t="n">
         <v>17935551439.9628</v>
       </c>
-      <c r="AS5" s="5" t="n">
+      <c r="AS5" s="10" t="n">
         <v>18867445497.8901</v>
       </c>
-      <c r="AT5" s="5" t="n">
+      <c r="AT5" s="10" t="n">
         <v>23346336999.4278</v>
       </c>
-      <c r="AU5" s="5" t="n">
+      <c r="AU5" s="10" t="n">
         <v>24202437752.744</v>
       </c>
-      <c r="AV5" s="5" t="n">
+      <c r="AV5" s="10" t="n">
         <v>23736144989.9615</v>
       </c>
-      <c r="AW5" s="5" t="n">
+      <c r="AW5" s="10" t="n">
         <v>28532797482.55</v>
       </c>
-      <c r="AX5" s="5"/>
+      <c r="AX5" s="10"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -3613,92 +3613,92 @@
       <c r="N6" t="s">
         <v>60</v>
       </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5" t="n">
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10" t="n">
         <v>2319508632</v>
       </c>
-      <c r="Z6" s="5" t="n">
+      <c r="Z6" s="10" t="n">
         <v>3862873021</v>
       </c>
-      <c r="AA6" s="5" t="n">
+      <c r="AA6" s="10" t="n">
         <v>6716695667</v>
       </c>
-      <c r="AB6" s="5" t="n">
+      <c r="AB6" s="10" t="n">
         <v>5826683842</v>
       </c>
-      <c r="AC6" s="5" t="n">
+      <c r="AC6" s="10" t="n">
         <v>6420590775.49</v>
       </c>
-      <c r="AD6" s="5" t="n">
+      <c r="AD6" s="10" t="n">
         <v>6663817369.9382</v>
       </c>
-      <c r="AE6" s="5" t="n">
+      <c r="AE6" s="10" t="n">
         <v>6681147280.0875</v>
       </c>
-      <c r="AF6" s="5" t="n">
+      <c r="AF6" s="10" t="n">
         <v>4732921597.2025</v>
       </c>
-      <c r="AG6" s="5" t="n">
+      <c r="AG6" s="10" t="n">
         <v>4721726624.2396</v>
       </c>
-      <c r="AH6" s="5" t="n">
+      <c r="AH6" s="10" t="n">
         <v>8546751672.1361</v>
       </c>
-      <c r="AI6" s="5" t="n">
+      <c r="AI6" s="10" t="n">
         <v>12943793441.7904</v>
       </c>
-      <c r="AJ6" s="5" t="n">
+      <c r="AJ6" s="10" t="n">
         <v>23517330173.7729</v>
       </c>
-      <c r="AK6" s="5" t="n">
+      <c r="AK6" s="10" t="n">
         <v>24143140491.499</v>
       </c>
-      <c r="AL6" s="5" t="n">
+      <c r="AL6" s="10" t="n">
         <v>28161849751.9937</v>
       </c>
-      <c r="AM6" s="5" t="n">
+      <c r="AM6" s="10" t="n">
         <v>23486898520.3541</v>
       </c>
-      <c r="AN6" s="5" t="n">
+      <c r="AN6" s="10" t="n">
         <v>24974244313.7798</v>
       </c>
-      <c r="AO6" s="5" t="n">
+      <c r="AO6" s="10" t="n">
         <v>24565223200.942</v>
       </c>
-      <c r="AP6" s="5" t="n">
+      <c r="AP6" s="10" t="n">
         <v>19926671669.1148</v>
       </c>
-      <c r="AQ6" s="5" t="n">
+      <c r="AQ6" s="10" t="n">
         <v>35369351064.3003</v>
       </c>
-      <c r="AR6" s="5" t="n">
+      <c r="AR6" s="10" t="n">
         <v>44571508294.1472</v>
       </c>
-      <c r="AS6" s="5" t="n">
+      <c r="AS6" s="10" t="n">
         <v>40847400896.9524</v>
       </c>
-      <c r="AT6" s="5" t="n">
+      <c r="AT6" s="10" t="n">
         <v>30275234223.2911</v>
       </c>
-      <c r="AU6" s="5" t="n">
+      <c r="AU6" s="10" t="n">
         <v>31600710295.201</v>
       </c>
-      <c r="AV6" s="5" t="n">
+      <c r="AV6" s="10" t="n">
         <v>54347517240.636</v>
       </c>
-      <c r="AW6" s="5" t="n">
+      <c r="AW6" s="10" t="n">
         <v>29096990570.6</v>
       </c>
-      <c r="AX6" s="5"/>
+      <c r="AX6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -3713,92 +3713,92 @@
       <c r="N7" t="s">
         <v>62</v>
       </c>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5" t="n">
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10" t="n">
         <v>33923574153.8018</v>
       </c>
-      <c r="Z7" s="5" t="n">
+      <c r="Z7" s="10" t="n">
         <v>37082616732.5682</v>
       </c>
-      <c r="AA7" s="5" t="n">
+      <c r="AA7" s="10" t="n">
         <v>41094385089.2003</v>
       </c>
-      <c r="AB7" s="5" t="n">
+      <c r="AB7" s="10" t="n">
         <v>51899640529.7878</v>
       </c>
-      <c r="AC7" s="5" t="n">
+      <c r="AC7" s="10" t="n">
         <v>61338691864.7592</v>
       </c>
-      <c r="AD7" s="5" t="n">
+      <c r="AD7" s="10" t="n">
         <v>63248753981.3984</v>
       </c>
-      <c r="AE7" s="5" t="n">
+      <c r="AE7" s="10" t="n">
         <v>68417078947.989</v>
       </c>
-      <c r="AF7" s="5" t="n">
+      <c r="AF7" s="10" t="n">
         <v>67886464978.9324</v>
       </c>
-      <c r="AG7" s="5" t="n">
+      <c r="AG7" s="10" t="n">
         <v>68195497229.5496</v>
       </c>
-      <c r="AH7" s="5" t="n">
+      <c r="AH7" s="10" t="n">
         <v>73116878071.4808</v>
       </c>
-      <c r="AI7" s="5" t="n">
+      <c r="AI7" s="10" t="n">
         <v>78737229887.1436</v>
       </c>
-      <c r="AJ7" s="5" t="n">
+      <c r="AJ7" s="10" t="n">
         <v>82973865635.6812</v>
       </c>
-      <c r="AK7" s="5" t="n">
+      <c r="AK7" s="10" t="n">
         <v>79353388215.7327</v>
       </c>
-      <c r="AL7" s="5" t="n">
+      <c r="AL7" s="10" t="n">
         <v>74840004095.2775</v>
       </c>
-      <c r="AM7" s="5" t="n">
+      <c r="AM7" s="10" t="n">
         <v>75370128901.0737</v>
       </c>
-      <c r="AN7" s="5" t="n">
+      <c r="AN7" s="10" t="n">
         <v>73951921579.6607</v>
       </c>
-      <c r="AO7" s="5" t="n">
+      <c r="AO7" s="10" t="n">
         <v>72437343715.4981</v>
       </c>
-      <c r="AP7" s="5" t="n">
+      <c r="AP7" s="10" t="n">
         <v>77152941104.441</v>
       </c>
-      <c r="AQ7" s="5" t="n">
+      <c r="AQ7" s="10" t="n">
         <v>74458064197.8283</v>
       </c>
-      <c r="AR7" s="5" t="n">
+      <c r="AR7" s="10" t="n">
         <v>81481014952.3075</v>
       </c>
-      <c r="AS7" s="5" t="n">
+      <c r="AS7" s="10" t="n">
         <v>81204255963.2088</v>
       </c>
-      <c r="AT7" s="5" t="n">
+      <c r="AT7" s="10" t="n">
         <v>82593624514.5921</v>
       </c>
-      <c r="AU7" s="5" t="n">
+      <c r="AU7" s="10" t="n">
         <v>87678852342.816</v>
       </c>
-      <c r="AV7" s="5" t="n">
+      <c r="AV7" s="10" t="n">
         <v>93248680100.8503</v>
       </c>
-      <c r="AW7" s="5" t="n">
+      <c r="AW7" s="10" t="n">
         <v>100393087198.87</v>
       </c>
-      <c r="AX7" s="5"/>
+      <c r="AX7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -3813,92 +3813,92 @@
       <c r="N8" t="s">
         <v>63</v>
       </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5" t="n">
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10" t="n">
         <v>5171873907.0695</v>
       </c>
-      <c r="Z8" s="5" t="n">
+      <c r="Z8" s="10" t="n">
         <v>4864881903.9802</v>
       </c>
-      <c r="AA8" s="5" t="n">
+      <c r="AA8" s="10" t="n">
         <v>6141425431.5808</v>
       </c>
-      <c r="AB8" s="5" t="n">
+      <c r="AB8" s="10" t="n">
         <v>8168326712.3567</v>
       </c>
-      <c r="AC8" s="5" t="n">
+      <c r="AC8" s="10" t="n">
         <v>9868043371.4774</v>
       </c>
-      <c r="AD8" s="5" t="n">
+      <c r="AD8" s="10" t="n">
         <v>11498663297.6905</v>
       </c>
-      <c r="AE8" s="5" t="n">
+      <c r="AE8" s="10" t="n">
         <v>14175256682.9303</v>
       </c>
-      <c r="AF8" s="5" t="n">
+      <c r="AF8" s="10" t="n">
         <v>15507929106.4192</v>
       </c>
-      <c r="AG8" s="5" t="n">
+      <c r="AG8" s="10" t="n">
         <v>17351555639.3725</v>
       </c>
-      <c r="AH8" s="5" t="n">
+      <c r="AH8" s="10" t="n">
         <v>16371231518.8311</v>
       </c>
-      <c r="AI8" s="5" t="n">
+      <c r="AI8" s="10" t="n">
         <v>16070266192.7763</v>
       </c>
-      <c r="AJ8" s="5" t="n">
+      <c r="AJ8" s="10" t="n">
         <v>11392985702.5436</v>
       </c>
-      <c r="AK8" s="5" t="n">
+      <c r="AK8" s="10" t="n">
         <v>8343721909.8577</v>
       </c>
-      <c r="AL8" s="5" t="n">
+      <c r="AL8" s="10" t="n">
         <v>4941324200.1482</v>
       </c>
-      <c r="AM8" s="5" t="n">
+      <c r="AM8" s="10" t="n">
         <v>2989748396.1557</v>
       </c>
-      <c r="AN8" s="5" t="n">
+      <c r="AN8" s="10" t="n">
         <v>2594164919.7514</v>
       </c>
-      <c r="AO8" s="5" t="n">
+      <c r="AO8" s="10" t="n">
         <v>2878470209.757</v>
       </c>
-      <c r="AP8" s="5" t="n">
+      <c r="AP8" s="10" t="n">
         <v>3157863136.3186</v>
       </c>
-      <c r="AQ8" s="5" t="n">
+      <c r="AQ8" s="10" t="n">
         <v>4603543026.0793</v>
       </c>
-      <c r="AR8" s="5" t="n">
+      <c r="AR8" s="10" t="n">
         <v>4274862144.6913</v>
       </c>
-      <c r="AS8" s="5" t="n">
+      <c r="AS8" s="10" t="n">
         <v>4355505138.7022</v>
       </c>
-      <c r="AT8" s="5" t="n">
+      <c r="AT8" s="10" t="n">
         <v>3787805557.1531</v>
       </c>
-      <c r="AU8" s="5" t="n">
+      <c r="AU8" s="10" t="n">
         <v>3768786244.3028</v>
       </c>
-      <c r="AV8" s="5" t="n">
+      <c r="AV8" s="10" t="n">
         <v>4907687338.1557</v>
       </c>
-      <c r="AW8" s="5" t="n">
+      <c r="AW8" s="10" t="n">
         <v>5527023886.1</v>
       </c>
-      <c r="AX8" s="5"/>
+      <c r="AX8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -3913,90 +3913,90 @@
       <c r="N9" t="s">
         <v>65</v>
       </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5" t="n">
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10" t="n">
         <v>5224643.8135</v>
       </c>
-      <c r="Z9" s="5" t="n">
+      <c r="Z9" s="10" t="n">
         <v>206279071.1</v>
       </c>
-      <c r="AA9" s="5" t="n">
+      <c r="AA9" s="10" t="n">
         <v>65968128.7305</v>
       </c>
-      <c r="AB9" s="5" t="n">
+      <c r="AB9" s="10" t="n">
         <v>202574519.3575</v>
       </c>
-      <c r="AC9" s="5" t="n">
+      <c r="AC9" s="10" t="n">
         <v>495140498.2077</v>
       </c>
-      <c r="AD9" s="5" t="n">
+      <c r="AD9" s="10" t="n">
         <v>1041052980.9954</v>
       </c>
-      <c r="AE9" s="5" t="n">
+      <c r="AE9" s="10" t="n">
         <v>3813647653.7202</v>
       </c>
-      <c r="AF9" s="5" t="n">
+      <c r="AF9" s="10" t="n">
         <v>18970921950.2802</v>
       </c>
-      <c r="AG9" s="5" t="n">
+      <c r="AG9" s="10" t="n">
         <v>27068236392.5027</v>
       </c>
-      <c r="AH9" s="5" t="n">
+      <c r="AH9" s="10" t="n">
         <v>33825821881.1283</v>
       </c>
-      <c r="AI9" s="5" t="n">
+      <c r="AI9" s="10" t="n">
         <v>568243791.9806</v>
       </c>
-      <c r="AJ9" s="5" t="n">
+      <c r="AJ9" s="10" t="n">
         <v>236279895.5134</v>
       </c>
-      <c r="AK9" s="5" t="n">
+      <c r="AK9" s="10" t="n">
         <v>-2993690.9378</v>
       </c>
-      <c r="AL9" s="5" t="n">
+      <c r="AL9" s="10" t="n">
         <v>-28841006.2989</v>
       </c>
-      <c r="AM9" s="5" t="n">
+      <c r="AM9" s="10" t="n">
         <v>-28331004.3713</v>
       </c>
-      <c r="AN9" s="5" t="n">
+      <c r="AN9" s="10" t="n">
         <v>186433.53</v>
       </c>
-      <c r="AO9" s="5" t="n">
+      <c r="AO9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AP9" s="5" t="n">
+      <c r="AP9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AQ9" s="5" t="n">
+      <c r="AQ9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AR9" s="5" t="n">
+      <c r="AR9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AS9" s="5" t="n">
+      <c r="AS9" s="10" t="n">
         <v>62886.3819</v>
       </c>
-      <c r="AT9" s="5" t="n">
+      <c r="AT9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AU9" s="5" t="n">
+      <c r="AU9" s="10" t="n">
         <v>467462</v>
       </c>
-      <c r="AV9" s="5"/>
-      <c r="AW9" s="5" t="n">
+      <c r="AV9" s="10"/>
+      <c r="AW9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AX9" s="5"/>
+      <c r="AX9" s="10"/>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -4011,92 +4011,92 @@
       <c r="N10" t="s">
         <v>66</v>
       </c>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5" t="n">
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10" t="n">
         <v>9177040538</v>
       </c>
-      <c r="Z10" s="5" t="n">
+      <c r="Z10" s="10" t="n">
         <v>10460196173.875</v>
       </c>
-      <c r="AA10" s="5" t="n">
+      <c r="AA10" s="10" t="n">
         <v>9441916441.72</v>
       </c>
-      <c r="AB10" s="5" t="n">
+      <c r="AB10" s="10" t="n">
         <v>10235455587.1225</v>
       </c>
-      <c r="AC10" s="5" t="n">
+      <c r="AC10" s="10" t="n">
         <v>11966493373.1891</v>
       </c>
-      <c r="AD10" s="5" t="n">
+      <c r="AD10" s="10" t="n">
         <v>12763119292.3131</v>
       </c>
-      <c r="AE10" s="5" t="n">
+      <c r="AE10" s="10" t="n">
         <v>16140443560.881</v>
       </c>
-      <c r="AF10" s="5" t="n">
+      <c r="AF10" s="10" t="n">
         <v>20400039840.0291</v>
       </c>
-      <c r="AG10" s="5" t="n">
+      <c r="AG10" s="10" t="n">
         <v>17378053458.7427</v>
       </c>
-      <c r="AH10" s="5" t="n">
+      <c r="AH10" s="10" t="n">
         <v>16622753232.4096</v>
       </c>
-      <c r="AI10" s="5" t="n">
+      <c r="AI10" s="10" t="n">
         <v>23392371164.3383</v>
       </c>
-      <c r="AJ10" s="5" t="n">
+      <c r="AJ10" s="10" t="n">
         <v>14851064502.5036</v>
       </c>
-      <c r="AK10" s="5" t="n">
+      <c r="AK10" s="10" t="n">
         <v>23337931129.3426</v>
       </c>
-      <c r="AL10" s="5" t="n">
+      <c r="AL10" s="10" t="n">
         <v>16367850469.2403</v>
       </c>
-      <c r="AM10" s="5" t="n">
+      <c r="AM10" s="10" t="n">
         <v>8248826567.2416</v>
       </c>
-      <c r="AN10" s="5" t="n">
+      <c r="AN10" s="10" t="n">
         <v>8437264592.828</v>
       </c>
-      <c r="AO10" s="5" t="n">
+      <c r="AO10" s="10" t="n">
         <v>25697143392.6293</v>
       </c>
-      <c r="AP10" s="5" t="n">
+      <c r="AP10" s="10" t="n">
         <v>37516349527.2804</v>
       </c>
-      <c r="AQ10" s="5" t="n">
+      <c r="AQ10" s="10" t="n">
         <v>38635685339.2009</v>
       </c>
-      <c r="AR10" s="5" t="n">
+      <c r="AR10" s="10" t="n">
         <v>31718734719.2681</v>
       </c>
-      <c r="AS10" s="5" t="n">
+      <c r="AS10" s="10" t="n">
         <v>52655095356.1555</v>
       </c>
-      <c r="AT10" s="5" t="n">
+      <c r="AT10" s="10" t="n">
         <v>23555050162.1593</v>
       </c>
-      <c r="AU10" s="5" t="n">
+      <c r="AU10" s="10" t="n">
         <v>27401777057.6908</v>
       </c>
-      <c r="AV10" s="5" t="n">
+      <c r="AV10" s="10" t="n">
         <v>32842452842.2362</v>
       </c>
-      <c r="AW10" s="5" t="n">
+      <c r="AW10" s="10" t="n">
         <v>39062361238.13</v>
       </c>
-      <c r="AX10" s="5"/>
+      <c r="AX10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -4109,112 +4109,112 @@
         <v>64</v>
       </c>
       <c r="N11"/>
-      <c r="O11" s="5" t="n">
+      <c r="O11" s="10" t="n">
         <v>120350129405</v>
       </c>
-      <c r="P11" s="5" t="n">
+      <c r="P11" s="10" t="n">
         <v>136154193844</v>
       </c>
-      <c r="Q11" s="5" t="n">
+      <c r="Q11" s="10" t="n">
         <v>123406660550</v>
       </c>
-      <c r="R11" s="5" t="n">
+      <c r="R11" s="10" t="n">
         <v>121373382142</v>
       </c>
-      <c r="S11" s="5" t="n">
+      <c r="S11" s="10" t="n">
         <v>117161902725</v>
       </c>
-      <c r="T11" s="5" t="n">
+      <c r="T11" s="10" t="n">
         <v>116592014868</v>
       </c>
-      <c r="U11" s="5" t="n">
+      <c r="U11" s="10" t="n">
         <v>118448779098</v>
       </c>
-      <c r="V11" s="5" t="n">
+      <c r="V11" s="10" t="n">
         <v>115982151879</v>
       </c>
-      <c r="W11" s="5" t="n">
+      <c r="W11" s="10" t="n">
         <v>116965882167</v>
       </c>
-      <c r="X11" s="5" t="n">
+      <c r="X11" s="10" t="n">
         <v>122185036488</v>
       </c>
-      <c r="Y11" s="5" t="n">
+      <c r="Y11" s="10" t="n">
         <v>12269320222.3246</v>
       </c>
-      <c r="Z11" s="5" t="n">
+      <c r="Z11" s="10" t="n">
         <v>6418404492.7689</v>
       </c>
-      <c r="AA11" s="5" t="n">
+      <c r="AA11" s="10" t="n">
         <v>8509751051.353</v>
       </c>
-      <c r="AB11" s="5" t="n">
+      <c r="AB11" s="10" t="n">
         <v>9084827512.3353</v>
       </c>
-      <c r="AC11" s="5" t="n">
+      <c r="AC11" s="10" t="n">
         <v>9270196138.4963</v>
       </c>
-      <c r="AD11" s="5" t="n">
+      <c r="AD11" s="10" t="n">
         <v>7410610517.917</v>
       </c>
-      <c r="AE11" s="5" t="n">
+      <c r="AE11" s="10" t="n">
         <v>4712411702.288</v>
       </c>
-      <c r="AF11" s="5" t="n">
+      <c r="AF11" s="10" t="n">
         <v>819783949.6251</v>
       </c>
-      <c r="AG11" s="5" t="n">
+      <c r="AG11" s="10" t="n">
         <v>6132864553.4893</v>
       </c>
-      <c r="AH11" s="5" t="n">
+      <c r="AH11" s="10" t="n">
         <v>3311213973.5083</v>
       </c>
-      <c r="AI11" s="5" t="n">
+      <c r="AI11" s="10" t="n">
         <v>1159366817.6825</v>
       </c>
-      <c r="AJ11" s="5" t="n">
+      <c r="AJ11" s="10" t="n">
         <v>1614694289.8918</v>
       </c>
-      <c r="AK11" s="5" t="n">
+      <c r="AK11" s="10" t="n">
         <v>3751512010.253</v>
       </c>
-      <c r="AL11" s="5" t="n">
+      <c r="AL11" s="10" t="n">
         <v>681354123.8563</v>
       </c>
-      <c r="AM11" s="5" t="n">
+      <c r="AM11" s="10" t="n">
         <v>821937209.9831</v>
       </c>
-      <c r="AN11" s="5" t="n">
+      <c r="AN11" s="10" t="n">
         <v>711366612.2216</v>
       </c>
-      <c r="AO11" s="5" t="n">
+      <c r="AO11" s="10" t="n">
         <v>727361939.5339</v>
       </c>
-      <c r="AP11" s="5" t="n">
+      <c r="AP11" s="10" t="n">
         <v>1145151354.4828</v>
       </c>
-      <c r="AQ11" s="5" t="n">
+      <c r="AQ11" s="10" t="n">
         <v>20204.7109</v>
       </c>
-      <c r="AR11" s="5" t="n">
+      <c r="AR11" s="10" t="n">
         <v>50903.5586</v>
       </c>
-      <c r="AS11" s="5" t="n">
+      <c r="AS11" s="10" t="n">
         <v>10000</v>
       </c>
-      <c r="AT11" s="5" t="n">
+      <c r="AT11" s="10" t="n">
         <v>10000</v>
       </c>
-      <c r="AU11" s="5" t="n">
+      <c r="AU11" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AV11" s="5" t="n">
+      <c r="AV11" s="10" t="n">
         <v>-29324.9492</v>
       </c>
-      <c r="AW11" s="5" t="n">
+      <c r="AW11" s="10" t="n">
         <v>10000</v>
       </c>
-      <c r="AX11" s="5"/>
+      <c r="AX11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -4229,112 +4229,112 @@
       <c r="N12" t="s">
         <v>21</v>
       </c>
-      <c r="O12" s="5" t="str">
+      <c r="O12" s="10" t="str">
         <f>Sum(O2:O11)</f>
       </c>
-      <c r="P12" s="5" t="str">
+      <c r="P12" s="10" t="str">
         <f>Sum(P2:P11)</f>
       </c>
-      <c r="Q12" s="5" t="str">
+      <c r="Q12" s="10" t="str">
         <f>Sum(Q2:Q11)</f>
       </c>
-      <c r="R12" s="5" t="str">
+      <c r="R12" s="10" t="str">
         <f>Sum(R2:R11)</f>
       </c>
-      <c r="S12" s="5" t="str">
+      <c r="S12" s="10" t="str">
         <f>Sum(S2:S11)</f>
       </c>
-      <c r="T12" s="5" t="str">
+      <c r="T12" s="10" t="str">
         <f>Sum(T2:T11)</f>
       </c>
-      <c r="U12" s="5" t="str">
+      <c r="U12" s="10" t="str">
         <f>Sum(U2:U11)</f>
       </c>
-      <c r="V12" s="5" t="str">
+      <c r="V12" s="10" t="str">
         <f>Sum(V2:V11)</f>
       </c>
-      <c r="W12" s="5" t="str">
+      <c r="W12" s="10" t="str">
         <f>Sum(W2:W11)</f>
       </c>
-      <c r="X12" s="5" t="str">
+      <c r="X12" s="10" t="str">
         <f>Sum(X2:X11)</f>
       </c>
-      <c r="Y12" s="5" t="str">
+      <c r="Y12" s="10" t="str">
         <f>Sum(Y2:Y11)</f>
       </c>
-      <c r="Z12" s="5" t="str">
+      <c r="Z12" s="10" t="str">
         <f>Sum(Z2:Z11)</f>
       </c>
-      <c r="AA12" s="5" t="str">
+      <c r="AA12" s="10" t="str">
         <f>Sum(AA2:AA11)</f>
       </c>
-      <c r="AB12" s="5" t="str">
+      <c r="AB12" s="10" t="str">
         <f>Sum(AB2:AB11)</f>
       </c>
-      <c r="AC12" s="5" t="str">
+      <c r="AC12" s="10" t="str">
         <f>Sum(AC2:AC11)</f>
       </c>
-      <c r="AD12" s="5" t="str">
+      <c r="AD12" s="10" t="str">
         <f>Sum(AD2:AD11)</f>
       </c>
-      <c r="AE12" s="5" t="str">
+      <c r="AE12" s="10" t="str">
         <f>Sum(AE2:AE11)</f>
       </c>
-      <c r="AF12" s="5" t="str">
+      <c r="AF12" s="10" t="str">
         <f>Sum(AF2:AF11)</f>
       </c>
-      <c r="AG12" s="5" t="str">
+      <c r="AG12" s="10" t="str">
         <f>Sum(AG2:AG11)</f>
       </c>
-      <c r="AH12" s="5" t="str">
+      <c r="AH12" s="10" t="str">
         <f>Sum(AH2:AH11)</f>
       </c>
-      <c r="AI12" s="5" t="str">
+      <c r="AI12" s="10" t="str">
         <f>Sum(AI2:AI11)</f>
       </c>
-      <c r="AJ12" s="5" t="str">
+      <c r="AJ12" s="10" t="str">
         <f>Sum(AJ2:AJ11)</f>
       </c>
-      <c r="AK12" s="5" t="str">
+      <c r="AK12" s="10" t="str">
         <f>Sum(AK2:AK11)</f>
       </c>
-      <c r="AL12" s="5" t="str">
+      <c r="AL12" s="10" t="str">
         <f>Sum(AL2:AL11)</f>
       </c>
-      <c r="AM12" s="5" t="str">
+      <c r="AM12" s="10" t="str">
         <f>Sum(AM2:AM11)</f>
       </c>
-      <c r="AN12" s="5" t="str">
+      <c r="AN12" s="10" t="str">
         <f>Sum(AN2:AN11)</f>
       </c>
-      <c r="AO12" s="5" t="str">
+      <c r="AO12" s="10" t="str">
         <f>Sum(AO2:AO11)</f>
       </c>
-      <c r="AP12" s="5" t="str">
+      <c r="AP12" s="10" t="str">
         <f>Sum(AP2:AP11)</f>
       </c>
-      <c r="AQ12" s="5" t="str">
+      <c r="AQ12" s="10" t="str">
         <f>Sum(AQ2:AQ11)</f>
       </c>
-      <c r="AR12" s="5" t="str">
+      <c r="AR12" s="10" t="str">
         <f>Sum(AR2:AR11)</f>
       </c>
-      <c r="AS12" s="5" t="str">
+      <c r="AS12" s="10" t="str">
         <f>Sum(AS2:AS11)</f>
       </c>
-      <c r="AT12" s="5" t="str">
+      <c r="AT12" s="10" t="str">
         <f>Sum(AT2:AT11)</f>
       </c>
-      <c r="AU12" s="5" t="str">
+      <c r="AU12" s="10" t="str">
         <f>Sum(AU2:AU11)</f>
       </c>
-      <c r="AV12" s="5" t="str">
+      <c r="AV12" s="10" t="str">
         <f>Sum(AV2:AV11)</f>
       </c>
-      <c r="AW12" s="5" t="str">
+      <c r="AW12" s="10" t="str">
         <f>Sum(AW2:AW11)</f>
       </c>
-      <c r="AX12" s="5"/>
+      <c r="AX12" s="10"/>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -4489,16 +4489,16 @@
       <c r="B16" t="str">
         <f>N16</f>
       </c>
-      <c r="C16" s="5" t="str">
+      <c r="C16" s="10" t="str">
         <f>AS16</f>
       </c>
-      <c r="D16" s="5" t="str">
+      <c r="D16" s="10" t="str">
         <f>AV16</f>
       </c>
-      <c r="E16" s="5" t="str">
+      <c r="E16" s="10" t="str">
         <f>AW16</f>
       </c>
-      <c r="F16" s="5" t="str">
+      <c r="F16" s="10" t="str">
         <f>AX16</f>
       </c>
       <c r="G16" s="2" t="str">
@@ -4522,92 +4522,92 @@
       <c r="N16" t="s">
         <v>55</v>
       </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="5" t="n">
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10" t="n">
         <v>99492846134.6049</v>
       </c>
-      <c r="Z16" s="5" t="n">
+      <c r="Z16" s="10" t="n">
         <v>111662179343.426</v>
       </c>
-      <c r="AA16" s="5" t="n">
+      <c r="AA16" s="10" t="n">
         <v>136020508440.748</v>
       </c>
-      <c r="AB16" s="5" t="n">
+      <c r="AB16" s="10" t="n">
         <v>173126078034.363</v>
       </c>
-      <c r="AC16" s="5" t="n">
+      <c r="AC16" s="10" t="n">
         <v>170122319818.576</v>
       </c>
-      <c r="AD16" s="5" t="n">
+      <c r="AD16" s="10" t="n">
         <v>192343869053.366</v>
       </c>
-      <c r="AE16" s="5" t="n">
+      <c r="AE16" s="10" t="n">
         <v>211882331398.365</v>
       </c>
-      <c r="AF16" s="5" t="n">
+      <c r="AF16" s="10" t="n">
         <v>236222162752.406</v>
       </c>
-      <c r="AG16" s="5" t="n">
+      <c r="AG16" s="10" t="n">
         <v>268639445187.611</v>
       </c>
-      <c r="AH16" s="5" t="n">
+      <c r="AH16" s="10" t="n">
         <v>240157851926.169</v>
       </c>
-      <c r="AI16" s="5" t="n">
+      <c r="AI16" s="10" t="n">
         <v>259984002918.056</v>
       </c>
-      <c r="AJ16" s="5" t="n">
+      <c r="AJ16" s="10" t="n">
         <v>247467219596.929</v>
       </c>
-      <c r="AK16" s="5" t="n">
+      <c r="AK16" s="10" t="n">
         <v>226017455664.798</v>
       </c>
-      <c r="AL16" s="5" t="n">
+      <c r="AL16" s="10" t="n">
         <v>188825337547.636</v>
       </c>
-      <c r="AM16" s="5" t="n">
+      <c r="AM16" s="10" t="n">
         <v>184279332054.837</v>
       </c>
-      <c r="AN16" s="5" t="n">
+      <c r="AN16" s="10" t="n">
         <v>176967438178.975</v>
       </c>
-      <c r="AO16" s="5" t="n">
+      <c r="AO16" s="10" t="n">
         <v>187531971552.558</v>
       </c>
-      <c r="AP16" s="5" t="n">
+      <c r="AP16" s="10" t="n">
         <v>191231821939.445</v>
       </c>
-      <c r="AQ16" s="5" t="n">
+      <c r="AQ16" s="10" t="n">
         <v>213890833618.391</v>
       </c>
-      <c r="AR16" s="5" t="n">
+      <c r="AR16" s="10" t="n">
         <v>226833952643.423</v>
       </c>
-      <c r="AS16" s="5" t="n">
+      <c r="AS16" s="10" t="n">
         <v>248629349244.482</v>
       </c>
-      <c r="AT16" s="5" t="n">
+      <c r="AT16" s="10" t="n">
         <v>237836959524.222</v>
       </c>
-      <c r="AU16" s="5" t="n">
+      <c r="AU16" s="10" t="n">
         <v>231405027838.097</v>
       </c>
-      <c r="AV16" s="5" t="n">
+      <c r="AV16" s="10" t="n">
         <v>229155776069.99</v>
       </c>
-      <c r="AW16" s="5" t="n">
+      <c r="AW16" s="10" t="n">
         <v>217527919786.283</v>
       </c>
-      <c r="AX16" s="5"/>
+      <c r="AX16" s="10"/>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -4616,16 +4616,16 @@
       <c r="B17" t="str">
         <f>N17</f>
       </c>
-      <c r="C17" s="5" t="str">
+      <c r="C17" s="10" t="str">
         <f>AS17</f>
       </c>
-      <c r="D17" s="5" t="str">
+      <c r="D17" s="10" t="str">
         <f>AV17</f>
       </c>
-      <c r="E17" s="5" t="str">
+      <c r="E17" s="10" t="str">
         <f>AW17</f>
       </c>
-      <c r="F17" s="5" t="str">
+      <c r="F17" s="10" t="str">
         <f>AX17</f>
       </c>
       <c r="G17" s="2" t="str">
@@ -4649,92 +4649,92 @@
       <c r="N17" t="s">
         <v>56</v>
       </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5" t="n">
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10" t="n">
         <v>9863413661.2718</v>
       </c>
-      <c r="Z17" s="5" t="n">
+      <c r="Z17" s="10" t="n">
         <v>13713864451.9095</v>
       </c>
-      <c r="AA17" s="5" t="n">
+      <c r="AA17" s="10" t="n">
         <v>13846410171.7735</v>
       </c>
-      <c r="AB17" s="5" t="n">
+      <c r="AB17" s="10" t="n">
         <v>14977255435.5173</v>
       </c>
-      <c r="AC17" s="5" t="n">
+      <c r="AC17" s="10" t="n">
         <v>17631870811.4125</v>
       </c>
-      <c r="AD17" s="5" t="n">
+      <c r="AD17" s="10" t="n">
         <v>33156013723.7303</v>
       </c>
-      <c r="AE17" s="5" t="n">
+      <c r="AE17" s="10" t="n">
         <v>28363332982.3688</v>
       </c>
-      <c r="AF17" s="5" t="n">
+      <c r="AF17" s="10" t="n">
         <v>24539151771.1166</v>
       </c>
-      <c r="AG17" s="5" t="n">
+      <c r="AG17" s="10" t="n">
         <v>31478447495.7358</v>
       </c>
-      <c r="AH17" s="5" t="n">
+      <c r="AH17" s="10" t="n">
         <v>33370208437.013</v>
       </c>
-      <c r="AI17" s="5" t="n">
+      <c r="AI17" s="10" t="n">
         <v>23367233101.6504</v>
       </c>
-      <c r="AJ17" s="5" t="n">
+      <c r="AJ17" s="10" t="n">
         <v>26175578966.1467</v>
       </c>
-      <c r="AK17" s="5" t="n">
+      <c r="AK17" s="10" t="n">
         <v>35538914515.196</v>
       </c>
-      <c r="AL17" s="5" t="n">
+      <c r="AL17" s="10" t="n">
         <v>23564363809.6933</v>
       </c>
-      <c r="AM17" s="5" t="n">
+      <c r="AM17" s="10" t="n">
         <v>14990252118.2584</v>
       </c>
-      <c r="AN17" s="5" t="n">
+      <c r="AN17" s="10" t="n">
         <v>11235130519.0313</v>
       </c>
-      <c r="AO17" s="5" t="n">
+      <c r="AO17" s="10" t="n">
         <v>9158533073.66965</v>
       </c>
-      <c r="AP17" s="5" t="n">
+      <c r="AP17" s="10" t="n">
         <v>11237830781.213</v>
       </c>
-      <c r="AQ17" s="5" t="n">
+      <c r="AQ17" s="10" t="n">
         <v>12520499886.2959</v>
       </c>
-      <c r="AR17" s="5" t="n">
+      <c r="AR17" s="10" t="n">
         <v>11431066234.3928</v>
       </c>
-      <c r="AS17" s="5" t="n">
+      <c r="AS17" s="10" t="n">
         <v>10276105861.5983</v>
       </c>
-      <c r="AT17" s="5" t="n">
+      <c r="AT17" s="10" t="n">
         <v>11592370968.9547</v>
       </c>
-      <c r="AU17" s="5" t="n">
+      <c r="AU17" s="10" t="n">
         <v>18317055457.9075</v>
       </c>
-      <c r="AV17" s="5" t="n">
+      <c r="AV17" s="10" t="n">
         <v>16776830306.481</v>
       </c>
-      <c r="AW17" s="5" t="n">
+      <c r="AW17" s="10" t="n">
         <v>16966395503.3249</v>
       </c>
-      <c r="AX17" s="5"/>
+      <c r="AX17" s="10"/>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -4743,16 +4743,16 @@
       <c r="B18" t="str">
         <f>N18</f>
       </c>
-      <c r="C18" s="5" t="str">
+      <c r="C18" s="10" t="str">
         <f>AS18</f>
       </c>
-      <c r="D18" s="5" t="str">
+      <c r="D18" s="10" t="str">
         <f>AV18</f>
       </c>
-      <c r="E18" s="5" t="str">
+      <c r="E18" s="10" t="str">
         <f>AW18</f>
       </c>
-      <c r="F18" s="5" t="str">
+      <c r="F18" s="10" t="str">
         <f>AX18</f>
       </c>
       <c r="G18" s="2" t="str">
@@ -4776,92 +4776,92 @@
       <c r="N18" t="s">
         <v>57</v>
       </c>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
-      <c r="Y18" s="5" t="n">
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10" t="n">
         <v>1635477886.47313</v>
       </c>
-      <c r="Z18" s="5" t="n">
+      <c r="Z18" s="10" t="n">
         <v>2578167591.81643</v>
       </c>
-      <c r="AA18" s="5" t="n">
+      <c r="AA18" s="10" t="n">
         <v>2834038617.46666</v>
       </c>
-      <c r="AB18" s="5" t="n">
+      <c r="AB18" s="10" t="n">
         <v>3371113908.85382</v>
       </c>
-      <c r="AC18" s="5" t="n">
+      <c r="AC18" s="10" t="n">
         <v>3748803153.68627</v>
       </c>
-      <c r="AD18" s="5" t="n">
+      <c r="AD18" s="10" t="n">
         <v>3746567923.6431</v>
       </c>
-      <c r="AE18" s="5" t="n">
+      <c r="AE18" s="10" t="n">
         <v>3432606776.97638</v>
       </c>
-      <c r="AF18" s="5" t="n">
+      <c r="AF18" s="10" t="n">
         <v>2390482488.56353</v>
       </c>
-      <c r="AG18" s="5" t="n">
+      <c r="AG18" s="10" t="n">
         <v>3750930032.25946</v>
       </c>
-      <c r="AH18" s="5" t="n">
+      <c r="AH18" s="10" t="n">
         <v>2484601525.90781</v>
       </c>
-      <c r="AI18" s="5" t="n">
+      <c r="AI18" s="10" t="n">
         <v>2490579965.96866</v>
       </c>
-      <c r="AJ18" s="5" t="n">
+      <c r="AJ18" s="10" t="n">
         <v>2586823625.15413</v>
       </c>
-      <c r="AK18" s="5" t="n">
+      <c r="AK18" s="10" t="n">
         <v>1599992442.63686</v>
       </c>
-      <c r="AL18" s="5" t="n">
+      <c r="AL18" s="10" t="n">
         <v>842812467.659801</v>
       </c>
-      <c r="AM18" s="5" t="n">
+      <c r="AM18" s="10" t="n">
         <v>597092301.092001</v>
       </c>
-      <c r="AN18" s="5" t="n">
+      <c r="AN18" s="10" t="n">
         <v>677822125.613794</v>
       </c>
-      <c r="AO18" s="5" t="n">
+      <c r="AO18" s="10" t="n">
         <v>689690760.751214</v>
       </c>
-      <c r="AP18" s="5" t="n">
+      <c r="AP18" s="10" t="n">
         <v>598605106.255239</v>
       </c>
-      <c r="AQ18" s="5" t="n">
+      <c r="AQ18" s="10" t="n">
         <v>525757862.476511</v>
       </c>
-      <c r="AR18" s="5" t="n">
+      <c r="AR18" s="10" t="n">
         <v>919840750.859922</v>
       </c>
-      <c r="AS18" s="5" t="n">
+      <c r="AS18" s="10" t="n">
         <v>1296661746.79702</v>
       </c>
-      <c r="AT18" s="5" t="n">
+      <c r="AT18" s="10" t="n">
         <v>1362434336.56837</v>
       </c>
-      <c r="AU18" s="5" t="n">
+      <c r="AU18" s="10" t="n">
         <v>1092822337.77335</v>
       </c>
-      <c r="AV18" s="5" t="n">
+      <c r="AV18" s="10" t="n">
         <v>1231672307.5974</v>
       </c>
-      <c r="AW18" s="5" t="n">
+      <c r="AW18" s="10" t="n">
         <v>1631323617.61389</v>
       </c>
-      <c r="AX18" s="5"/>
+      <c r="AX18" s="10"/>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -4870,16 +4870,16 @@
       <c r="B19" t="str">
         <f>N19</f>
       </c>
-      <c r="C19" s="5" t="str">
+      <c r="C19" s="10" t="str">
         <f>AS19</f>
       </c>
-      <c r="D19" s="5" t="str">
+      <c r="D19" s="10" t="str">
         <f>AV19</f>
       </c>
-      <c r="E19" s="5" t="str">
+      <c r="E19" s="10" t="str">
         <f>AW19</f>
       </c>
-      <c r="F19" s="5" t="str">
+      <c r="F19" s="10" t="str">
         <f>AX19</f>
       </c>
       <c r="G19" s="2" t="str">
@@ -4903,92 +4903,92 @@
       <c r="N19" t="s">
         <v>59</v>
       </c>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
-      <c r="Y19" s="5" t="n">
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10" t="n">
         <v>5533658963.28193</v>
       </c>
-      <c r="Z19" s="5" t="n">
+      <c r="Z19" s="10" t="n">
         <v>5159680279.02277</v>
       </c>
-      <c r="AA19" s="5" t="n">
+      <c r="AA19" s="10" t="n">
         <v>5405676449.56396</v>
       </c>
-      <c r="AB19" s="5" t="n">
+      <c r="AB19" s="10" t="n">
         <v>8485660038.90305</v>
       </c>
-      <c r="AC19" s="5" t="n">
+      <c r="AC19" s="10" t="n">
         <v>10346454163.9903</v>
       </c>
-      <c r="AD19" s="5" t="n">
+      <c r="AD19" s="10" t="n">
         <v>15642313416.8038</v>
       </c>
-      <c r="AE19" s="5" t="n">
+      <c r="AE19" s="10" t="n">
         <v>19963252117.6419</v>
       </c>
-      <c r="AF19" s="5" t="n">
+      <c r="AF19" s="10" t="n">
         <v>19775883870.797</v>
       </c>
-      <c r="AG19" s="5" t="n">
+      <c r="AG19" s="10" t="n">
         <v>25044918515.4242</v>
       </c>
-      <c r="AH19" s="5" t="n">
+      <c r="AH19" s="10" t="n">
         <v>20348495570.0175</v>
       </c>
-      <c r="AI19" s="5" t="n">
+      <c r="AI19" s="10" t="n">
         <v>26989883007.2929</v>
       </c>
-      <c r="AJ19" s="5" t="n">
+      <c r="AJ19" s="10" t="n">
         <v>35987539559.4035</v>
       </c>
-      <c r="AK19" s="5" t="n">
+      <c r="AK19" s="10" t="n">
         <v>23691892482.563</v>
       </c>
-      <c r="AL19" s="5" t="n">
+      <c r="AL19" s="10" t="n">
         <v>22675351533.7461</v>
       </c>
-      <c r="AM19" s="5" t="n">
+      <c r="AM19" s="10" t="n">
         <v>18282033036.7687</v>
       </c>
-      <c r="AN19" s="5" t="n">
+      <c r="AN19" s="10" t="n">
         <v>15767151181.1605</v>
       </c>
-      <c r="AO19" s="5" t="n">
+      <c r="AO19" s="10" t="n">
         <v>16396513530.6887</v>
       </c>
-      <c r="AP19" s="5" t="n">
+      <c r="AP19" s="10" t="n">
         <v>20266253467.0279</v>
       </c>
-      <c r="AQ19" s="5" t="n">
+      <c r="AQ19" s="10" t="n">
         <v>18783352376.9608</v>
       </c>
-      <c r="AR19" s="5" t="n">
+      <c r="AR19" s="10" t="n">
         <v>21029610653.8864</v>
       </c>
-      <c r="AS19" s="5" t="n">
+      <c r="AS19" s="10" t="n">
         <v>21837006462.3676</v>
       </c>
-      <c r="AT19" s="5" t="n">
+      <c r="AT19" s="10" t="n">
         <v>26121790628.0107</v>
       </c>
-      <c r="AU19" s="5" t="n">
+      <c r="AU19" s="10" t="n">
         <v>25309616863.8217</v>
       </c>
-      <c r="AV19" s="5" t="n">
+      <c r="AV19" s="10" t="n">
         <v>23736144989.9615</v>
       </c>
-      <c r="AW19" s="5" t="n">
+      <c r="AW19" s="10" t="n">
         <v>27790621478.824</v>
       </c>
-      <c r="AX19" s="5"/>
+      <c r="AX19" s="10"/>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -4997,16 +4997,16 @@
       <c r="B20" t="str">
         <f>N20</f>
       </c>
-      <c r="C20" s="5" t="str">
+      <c r="C20" s="10" t="str">
         <f>AS20</f>
       </c>
-      <c r="D20" s="5" t="str">
+      <c r="D20" s="10" t="str">
         <f>AV20</f>
       </c>
-      <c r="E20" s="5" t="str">
+      <c r="E20" s="10" t="str">
         <f>AW20</f>
       </c>
-      <c r="F20" s="5" t="str">
+      <c r="F20" s="10" t="str">
         <f>AX20</f>
       </c>
       <c r="G20" s="2" t="str">
@@ -5030,92 +5030,92 @@
       <c r="N20" t="s">
         <v>60</v>
       </c>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-      <c r="V20" s="5"/>
-      <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
-      <c r="Y20" s="5" t="n">
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10" t="n">
         <v>3899496193.18712</v>
       </c>
-      <c r="Z20" s="5" t="n">
+      <c r="Z20" s="10" t="n">
         <v>6340472090.99328</v>
       </c>
-      <c r="AA20" s="5" t="n">
+      <c r="AA20" s="10" t="n">
         <v>10853945463.6745</v>
       </c>
-      <c r="AB20" s="5" t="n">
+      <c r="AB20" s="10" t="n">
         <v>9238385454.51997</v>
       </c>
-      <c r="AC20" s="5" t="n">
+      <c r="AC20" s="10" t="n">
         <v>9937384506.12464</v>
       </c>
-      <c r="AD20" s="5" t="n">
+      <c r="AD20" s="10" t="n">
         <v>10009255405.2905</v>
       </c>
-      <c r="AE20" s="5" t="n">
+      <c r="AE20" s="10" t="n">
         <v>9719552474.71939</v>
       </c>
-      <c r="AF20" s="5" t="n">
+      <c r="AF20" s="10" t="n">
         <v>6700855248.30451</v>
       </c>
-      <c r="AG20" s="5" t="n">
+      <c r="AG20" s="10" t="n">
         <v>6549041799.65516</v>
       </c>
-      <c r="AH20" s="5" t="n">
+      <c r="AH20" s="10" t="n">
         <v>11734360319.6467</v>
       </c>
-      <c r="AI20" s="5" t="n">
+      <c r="AI20" s="10" t="n">
         <v>17618742917.7099</v>
       </c>
-      <c r="AJ20" s="5" t="n">
+      <c r="AJ20" s="10" t="n">
         <v>31381290950.4757</v>
       </c>
-      <c r="AK20" s="5" t="n">
+      <c r="AK20" s="10" t="n">
         <v>31642185537.1118</v>
       </c>
-      <c r="AL20" s="5" t="n">
+      <c r="AL20" s="10" t="n">
         <v>36251365581.0423</v>
       </c>
-      <c r="AM20" s="5" t="n">
+      <c r="AM20" s="10" t="n">
         <v>29691856901.7663</v>
       </c>
-      <c r="AN20" s="5" t="n">
+      <c r="AN20" s="10" t="n">
         <v>31248524019.3981</v>
       </c>
-      <c r="AO20" s="5" t="n">
+      <c r="AO20" s="10" t="n">
         <v>30492950960.1538</v>
       </c>
-      <c r="AP20" s="5" t="n">
+      <c r="AP20" s="10" t="n">
         <v>24324488111.1612</v>
       </c>
-      <c r="AQ20" s="5" t="n">
+      <c r="AQ20" s="10" t="n">
         <v>42237690109.0382</v>
       </c>
-      <c r="AR20" s="5" t="n">
+      <c r="AR20" s="10" t="n">
         <v>52260532318.728</v>
       </c>
-      <c r="AS20" s="5" t="n">
+      <c r="AS20" s="10" t="n">
         <v>47276403022.2014</v>
       </c>
-      <c r="AT20" s="5" t="n">
+      <c r="AT20" s="10" t="n">
         <v>33874407347.6785</v>
       </c>
-      <c r="AU20" s="5" t="n">
+      <c r="AU20" s="10" t="n">
         <v>33046335181.8965</v>
       </c>
-      <c r="AV20" s="5" t="n">
+      <c r="AV20" s="10" t="n">
         <v>54347517240.636</v>
       </c>
-      <c r="AW20" s="5" t="n">
+      <c r="AW20" s="10" t="n">
         <v>28340139154.4236</v>
       </c>
-      <c r="AX20" s="5"/>
+      <c r="AX20" s="10"/>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -5124,16 +5124,16 @@
       <c r="B21" t="str">
         <f>N21</f>
       </c>
-      <c r="C21" s="5" t="str">
+      <c r="C21" s="10" t="str">
         <f>AS21</f>
       </c>
-      <c r="D21" s="5" t="str">
+      <c r="D21" s="10" t="str">
         <f>AV21</f>
       </c>
-      <c r="E21" s="5" t="str">
+      <c r="E21" s="10" t="str">
         <f>AW21</f>
       </c>
-      <c r="F21" s="5" t="str">
+      <c r="F21" s="10" t="str">
         <f>AX21</f>
       </c>
       <c r="G21" s="2" t="str">
@@ -5157,92 +5157,92 @@
       <c r="N21" t="s">
         <v>62</v>
       </c>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
-      <c r="Y21" s="5" t="n">
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10" t="n">
         <v>57031410207.7681</v>
       </c>
-      <c r="Z21" s="5" t="n">
+      <c r="Z21" s="10" t="n">
         <v>60866949334.2502</v>
       </c>
-      <c r="AA21" s="5" t="n">
+      <c r="AA21" s="10" t="n">
         <v>66407090142.9782</v>
       </c>
-      <c r="AB21" s="5" t="n">
+      <c r="AB21" s="10" t="n">
         <v>82288467534.3273</v>
       </c>
-      <c r="AC21" s="5" t="n">
+      <c r="AC21" s="10" t="n">
         <v>94936149565.8151</v>
       </c>
-      <c r="AD21" s="5" t="n">
+      <c r="AD21" s="10" t="n">
         <v>95001543037.7971</v>
       </c>
-      <c r="AE21" s="5" t="n">
+      <c r="AE21" s="10" t="n">
         <v>99531317171.2164</v>
       </c>
-      <c r="AF21" s="5" t="n">
+      <c r="AF21" s="10" t="n">
         <v>96113439827.9061</v>
       </c>
-      <c r="AG21" s="5" t="n">
+      <c r="AG21" s="10" t="n">
         <v>94587255351.0047</v>
       </c>
-      <c r="AH21" s="5" t="n">
+      <c r="AH21" s="10" t="n">
         <v>100386652807.007</v>
       </c>
-      <c r="AI21" s="5" t="n">
+      <c r="AI21" s="10" t="n">
         <v>107174996083.862</v>
       </c>
-      <c r="AJ21" s="5" t="n">
+      <c r="AJ21" s="10" t="n">
         <v>110719499176.094</v>
       </c>
-      <c r="AK21" s="5" t="n">
+      <c r="AK21" s="10" t="n">
         <v>104001160652.848</v>
       </c>
-      <c r="AL21" s="5" t="n">
+      <c r="AL21" s="10" t="n">
         <v>96337860347.8465</v>
       </c>
-      <c r="AM21" s="5" t="n">
+      <c r="AM21" s="10" t="n">
         <v>95282017762.3275</v>
       </c>
-      <c r="AN21" s="5" t="n">
+      <c r="AN21" s="10" t="n">
         <v>92530863746.2001</v>
       </c>
-      <c r="AO21" s="5" t="n">
+      <c r="AO21" s="10" t="n">
         <v>89916885815.871</v>
       </c>
-      <c r="AP21" s="5" t="n">
+      <c r="AP21" s="10" t="n">
         <v>94180595224.2832</v>
       </c>
-      <c r="AQ21" s="5" t="n">
+      <c r="AQ21" s="10" t="n">
         <v>88917001501.9319</v>
       </c>
-      <c r="AR21" s="5" t="n">
+      <c r="AR21" s="10" t="n">
         <v>95537292280.4362</v>
       </c>
-      <c r="AS21" s="5" t="n">
+      <c r="AS21" s="10" t="n">
         <v>93985052848.7624</v>
       </c>
-      <c r="AT21" s="5" t="n">
+      <c r="AT21" s="10" t="n">
         <v>92412499949.4177</v>
       </c>
-      <c r="AU21" s="5" t="n">
+      <c r="AU21" s="10" t="n">
         <v>91689861266.3376</v>
       </c>
-      <c r="AV21" s="5" t="n">
+      <c r="AV21" s="10" t="n">
         <v>93248680100.8503</v>
       </c>
-      <c r="AW21" s="5" t="n">
+      <c r="AW21" s="10" t="n">
         <v>97781729504.1139</v>
       </c>
-      <c r="AX21" s="5"/>
+      <c r="AX21" s="10"/>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -5251,16 +5251,16 @@
       <c r="B22" t="str">
         <f>N22</f>
       </c>
-      <c r="C22" s="5" t="str">
+      <c r="C22" s="10" t="str">
         <f>AS22</f>
       </c>
-      <c r="D22" s="5" t="str">
+      <c r="D22" s="10" t="str">
         <f>AV22</f>
       </c>
-      <c r="E22" s="5" t="str">
+      <c r="E22" s="10" t="str">
         <f>AW22</f>
       </c>
-      <c r="F22" s="5" t="str">
+      <c r="F22" s="10" t="str">
         <f>AX22</f>
       </c>
       <c r="G22" s="2" t="str">
@@ -5284,92 +5284,92 @@
       <c r="N22" t="s">
         <v>63</v>
       </c>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
-      <c r="Y22" s="5" t="n">
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10" t="n">
         <v>8694816796.12103</v>
       </c>
-      <c r="Z22" s="5" t="n">
+      <c r="Z22" s="10" t="n">
         <v>7985157102.10416</v>
       </c>
-      <c r="AA22" s="5" t="n">
+      <c r="AA22" s="10" t="n">
         <v>9924328867.7057</v>
       </c>
-      <c r="AB22" s="5" t="n">
+      <c r="AB22" s="10" t="n">
         <v>12951131850.2053</v>
       </c>
-      <c r="AC22" s="5" t="n">
+      <c r="AC22" s="10" t="n">
         <v>15273133693.5271</v>
       </c>
-      <c r="AD22" s="5" t="n">
+      <c r="AD22" s="10" t="n">
         <v>17271340340.9331</v>
       </c>
-      <c r="AE22" s="5" t="n">
+      <c r="AE22" s="10" t="n">
         <v>20621780271.6292</v>
       </c>
-      <c r="AF22" s="5" t="n">
+      <c r="AF22" s="10" t="n">
         <v>21956076391.4842</v>
       </c>
-      <c r="AG22" s="5" t="n">
+      <c r="AG22" s="10" t="n">
         <v>24066633292.1367</v>
       </c>
-      <c r="AH22" s="5" t="n">
+      <c r="AH22" s="10" t="n">
         <v>22477069287.5774</v>
       </c>
-      <c r="AI22" s="5" t="n">
+      <c r="AI22" s="10" t="n">
         <v>21874413396.8911</v>
       </c>
-      <c r="AJ22" s="5" t="n">
+      <c r="AJ22" s="10" t="n">
         <v>15202686550.0597</v>
       </c>
-      <c r="AK22" s="5" t="n">
+      <c r="AK22" s="10" t="n">
         <v>10935346080.3802</v>
       </c>
-      <c r="AL22" s="5" t="n">
+      <c r="AL22" s="10" t="n">
         <v>6360723873.30816</v>
       </c>
-      <c r="AM22" s="5" t="n">
+      <c r="AM22" s="10" t="n">
         <v>3779604253.58035</v>
       </c>
-      <c r="AN22" s="5" t="n">
+      <c r="AN22" s="10" t="n">
         <v>3245897004.39519</v>
       </c>
-      <c r="AO22" s="5" t="n">
+      <c r="AO22" s="10" t="n">
         <v>3573061405.89099</v>
       </c>
-      <c r="AP22" s="5" t="n">
+      <c r="AP22" s="10" t="n">
         <v>3854803531.24462</v>
       </c>
-      <c r="AQ22" s="5" t="n">
+      <c r="AQ22" s="10" t="n">
         <v>5497500459.8097</v>
       </c>
-      <c r="AR22" s="5" t="n">
+      <c r="AR22" s="10" t="n">
         <v>5012317954.24977</v>
       </c>
-      <c r="AS22" s="5" t="n">
+      <c r="AS22" s="10" t="n">
         <v>5041021259.14986</v>
       </c>
-      <c r="AT22" s="5" t="n">
+      <c r="AT22" s="10" t="n">
         <v>4238106547.76353</v>
       </c>
-      <c r="AU22" s="5" t="n">
+      <c r="AU22" s="10" t="n">
         <v>3941195381.20207</v>
       </c>
-      <c r="AV22" s="5" t="n">
+      <c r="AV22" s="10" t="n">
         <v>4907687338.1557</v>
       </c>
-      <c r="AW22" s="5" t="n">
+      <c r="AW22" s="10" t="n">
         <v>5383258645.31726</v>
       </c>
-      <c r="AX22" s="5"/>
+      <c r="AX22" s="10"/>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -5378,16 +5378,16 @@
       <c r="B23" t="str">
         <f>N23</f>
       </c>
-      <c r="C23" s="5" t="str">
+      <c r="C23" s="10" t="str">
         <f>AS23</f>
       </c>
-      <c r="D23" s="5" t="str">
+      <c r="D23" s="10" t="str">
         <f>AV23</f>
       </c>
-      <c r="E23" s="5" t="str">
+      <c r="E23" s="10" t="str">
         <f>AW23</f>
       </c>
-      <c r="F23" s="5" t="str">
+      <c r="F23" s="10" t="str">
         <f>AX23</f>
       </c>
       <c r="G23" s="2" t="str">
@@ -5411,90 +5411,90 @@
       <c r="N23" t="s">
         <v>65</v>
       </c>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5" t="n">
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10" t="n">
         <v>8783532.15867742</v>
       </c>
-      <c r="Z23" s="5" t="n">
+      <c r="Z23" s="10" t="n">
         <v>338583920.868045</v>
       </c>
-      <c r="AA23" s="5" t="n">
+      <c r="AA23" s="10" t="n">
         <v>106602190.582995</v>
       </c>
-      <c r="AB23" s="5" t="n">
+      <c r="AB23" s="10" t="n">
         <v>321188096.666375</v>
       </c>
-      <c r="AC23" s="5" t="n">
+      <c r="AC23" s="10" t="n">
         <v>766347161.39007</v>
       </c>
-      <c r="AD23" s="5" t="n">
+      <c r="AD23" s="10" t="n">
         <v>1563693090.42434</v>
       </c>
-      <c r="AE23" s="5" t="n">
+      <c r="AE23" s="10" t="n">
         <v>5547991525.48221</v>
       </c>
-      <c r="AF23" s="5" t="n">
+      <c r="AF23" s="10" t="n">
         <v>26858970575.5634</v>
       </c>
-      <c r="AG23" s="5" t="n">
+      <c r="AG23" s="10" t="n">
         <v>37543683843.8302</v>
       </c>
-      <c r="AH23" s="5" t="n">
+      <c r="AH23" s="10" t="n">
         <v>46441548472.1981</v>
       </c>
-      <c r="AI23" s="5" t="n">
+      <c r="AI23" s="10" t="n">
         <v>773478140.740941</v>
       </c>
-      <c r="AJ23" s="5" t="n">
+      <c r="AJ23" s="10" t="n">
         <v>315289537.20789</v>
       </c>
-      <c r="AK23" s="5" t="n">
+      <c r="AK23" s="10" t="n">
         <v>-3923554.35814127</v>
       </c>
-      <c r="AL23" s="5" t="n">
+      <c r="AL23" s="10" t="n">
         <v>-37125610.4365996</v>
       </c>
-      <c r="AM23" s="5" t="n">
+      <c r="AM23" s="10" t="n">
         <v>-35815717.7265001</v>
       </c>
-      <c r="AN23" s="5" t="n">
+      <c r="AN23" s="10" t="n">
         <v>233271.228031182</v>
       </c>
-      <c r="AO23" s="5" t="n">
+      <c r="AO23" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AP23" s="5" t="n">
+      <c r="AP23" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AQ23" s="5" t="n">
+      <c r="AQ23" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AR23" s="5" t="n">
+      <c r="AR23" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AS23" s="5" t="n">
+      <c r="AS23" s="10" t="n">
         <v>72784.1152687462</v>
       </c>
-      <c r="AT23" s="5" t="n">
+      <c r="AT23" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AU23" s="5" t="n">
+      <c r="AU23" s="10" t="n">
         <v>488846.794660361</v>
       </c>
-      <c r="AV23" s="5"/>
-      <c r="AW23" s="5" t="n">
+      <c r="AV23" s="10"/>
+      <c r="AW23" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AX23" s="5"/>
+      <c r="AX23" s="10"/>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -5503,16 +5503,16 @@
       <c r="B24" t="str">
         <f>N24</f>
       </c>
-      <c r="C24" s="5" t="str">
+      <c r="C24" s="10" t="str">
         <f>AS24</f>
       </c>
-      <c r="D24" s="5" t="str">
+      <c r="D24" s="10" t="str">
         <f>AV24</f>
       </c>
-      <c r="E24" s="5" t="str">
+      <c r="E24" s="10" t="str">
         <f>AW24</f>
       </c>
-      <c r="F24" s="5" t="str">
+      <c r="F24" s="10" t="str">
         <f>AX24</f>
       </c>
       <c r="G24" s="2" t="str">
@@ -5536,92 +5536,92 @@
       <c r="N24" t="s">
         <v>66</v>
       </c>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5" t="n">
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10" t="n">
         <v>15428196364.0715</v>
       </c>
-      <c r="Z24" s="5" t="n">
+      <c r="Z24" s="10" t="n">
         <v>17169236872.715</v>
       </c>
-      <c r="AA24" s="5" t="n">
+      <c r="AA24" s="10" t="n">
         <v>15257806994.9646</v>
       </c>
-      <c r="AB24" s="5" t="n">
+      <c r="AB24" s="10" t="n">
         <v>16228627909.2158</v>
       </c>
-      <c r="AC24" s="5" t="n">
+      <c r="AC24" s="10" t="n">
         <v>18520981946.6024</v>
       </c>
-      <c r="AD24" s="5" t="n">
+      <c r="AD24" s="10" t="n">
         <v>19170591520.2982</v>
       </c>
-      <c r="AE24" s="5" t="n">
+      <c r="AE24" s="10" t="n">
         <v>23480681023.5704</v>
       </c>
-      <c r="AF24" s="5" t="n">
+      <c r="AF24" s="10" t="n">
         <v>28882311109.5857</v>
       </c>
-      <c r="AG24" s="5" t="n">
+      <c r="AG24" s="10" t="n">
         <v>24103385806.7283</v>
       </c>
-      <c r="AH24" s="5" t="n">
+      <c r="AH24" s="10" t="n">
         <v>22822398896.8332</v>
       </c>
-      <c r="AI24" s="5" t="n">
+      <c r="AI24" s="10" t="n">
         <v>31841065421.322</v>
       </c>
-      <c r="AJ24" s="5" t="n">
+      <c r="AJ24" s="10" t="n">
         <v>19817112428.7353</v>
       </c>
-      <c r="AK24" s="5" t="n">
+      <c r="AK24" s="10" t="n">
         <v>30586871956.7371</v>
       </c>
-      <c r="AL24" s="5" t="n">
+      <c r="AL24" s="10" t="n">
         <v>21069529748.9917</v>
       </c>
-      <c r="AM24" s="5" t="n">
+      <c r="AM24" s="10" t="n">
         <v>10428068134.6569</v>
       </c>
-      <c r="AN24" s="5" t="n">
+      <c r="AN24" s="10" t="n">
         <v>10556958680.0883</v>
       </c>
-      <c r="AO24" s="5" t="n">
+      <c r="AO24" s="10" t="n">
         <v>31898009917.4282</v>
       </c>
-      <c r="AP24" s="5" t="n">
+      <c r="AP24" s="10" t="n">
         <v>45796207876.7486</v>
       </c>
-      <c r="AQ24" s="5" t="n">
+      <c r="AQ24" s="10" t="n">
         <v>46138310582.5372</v>
       </c>
-      <c r="AR24" s="5" t="n">
+      <c r="AR24" s="10" t="n">
         <v>37190528755.8586</v>
       </c>
-      <c r="AS24" s="5" t="n">
+      <c r="AS24" s="10" t="n">
         <v>60942519097.1154</v>
       </c>
-      <c r="AT24" s="5" t="n">
+      <c r="AT24" s="10" t="n">
         <v>26355315978.832</v>
       </c>
-      <c r="AU24" s="5" t="n">
+      <c r="AU24" s="10" t="n">
         <v>28655315047.3193</v>
       </c>
-      <c r="AV24" s="5" t="n">
+      <c r="AV24" s="10" t="n">
         <v>32842452842.2362</v>
       </c>
-      <c r="AW24" s="5" t="n">
+      <c r="AW24" s="10" t="n">
         <v>38046297279.5382</v>
       </c>
-      <c r="AX24" s="5"/>
+      <c r="AX24" s="10"/>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -5630,16 +5630,16 @@
       <c r="B25" t="str">
         <f>N25</f>
       </c>
-      <c r="C25" s="5" t="str">
+      <c r="C25" s="10" t="str">
         <f>AS25</f>
       </c>
-      <c r="D25" s="5" t="str">
+      <c r="D25" s="10" t="str">
         <f>AV25</f>
       </c>
-      <c r="E25" s="5" t="str">
+      <c r="E25" s="10" t="str">
         <f>AW25</f>
       </c>
-      <c r="F25" s="5" t="str">
+      <c r="F25" s="10" t="str">
         <f>AX25</f>
       </c>
       <c r="G25" s="2" t="str">
@@ -5661,112 +5661,112 @@
         <v>64</v>
       </c>
       <c r="N25"/>
-      <c r="O25" s="5" t="n">
+      <c r="O25" s="10" t="n">
         <v>248917998790.874</v>
       </c>
-      <c r="P25" s="5" t="n">
+      <c r="P25" s="10" t="n">
         <v>271885202720.129</v>
       </c>
-      <c r="Q25" s="5" t="n">
+      <c r="Q25" s="10" t="n">
         <v>240412560734.939</v>
       </c>
-      <c r="R25" s="5" t="n">
+      <c r="R25" s="10" t="n">
         <v>231031479111.987</v>
       </c>
-      <c r="S25" s="5" t="n">
+      <c r="S25" s="10" t="n">
         <v>218250472650.085</v>
       </c>
-      <c r="T25" s="5" t="n">
+      <c r="T25" s="10" t="n">
         <v>212677633977.603</v>
       </c>
-      <c r="U25" s="5" t="n">
+      <c r="U25" s="10" t="n">
         <v>212071611328.834</v>
       </c>
-      <c r="V25" s="5" t="n">
+      <c r="V25" s="10" t="n">
         <v>204034317412.979</v>
       </c>
-      <c r="W25" s="5" t="n">
+      <c r="W25" s="10" t="n">
         <v>203216983313.484</v>
       </c>
-      <c r="X25" s="5" t="n">
+      <c r="X25" s="10" t="n">
         <v>209688280565.4</v>
       </c>
-      <c r="Y25" s="5" t="n">
+      <c r="Y25" s="10" t="n">
         <v>20626854688.053</v>
       </c>
-      <c r="Z25" s="5" t="n">
+      <c r="Z25" s="10" t="n">
         <v>10535089901.7053</v>
       </c>
-      <c r="AA25" s="5" t="n">
+      <c r="AA25" s="10" t="n">
         <v>13751460301.3251</v>
       </c>
-      <c r="AB25" s="5" t="n">
+      <c r="AB25" s="10" t="n">
         <v>14404271901.9353</v>
       </c>
-      <c r="AC25" s="5" t="n">
+      <c r="AC25" s="10" t="n">
         <v>14347823540.9574</v>
       </c>
-      <c r="AD25" s="5" t="n">
+      <c r="AD25" s="10" t="n">
         <v>11130961319.1953</v>
       </c>
-      <c r="AE25" s="5" t="n">
+      <c r="AE25" s="10" t="n">
         <v>6855489170.15793</v>
       </c>
-      <c r="AF25" s="5" t="n">
+      <c r="AF25" s="10" t="n">
         <v>1160647491.93565</v>
       </c>
-      <c r="AG25" s="5" t="n">
+      <c r="AG25" s="10" t="n">
         <v>8506292191.13106</v>
       </c>
-      <c r="AH25" s="5" t="n">
+      <c r="AH25" s="10" t="n">
         <v>4546169041.89102</v>
       </c>
-      <c r="AI25" s="5" t="n">
+      <c r="AI25" s="10" t="n">
         <v>1578098878.04004</v>
       </c>
-      <c r="AJ25" s="5" t="n">
+      <c r="AJ25" s="10" t="n">
         <v>2154631964.28973</v>
       </c>
-      <c r="AK25" s="5" t="n">
+      <c r="AK25" s="10" t="n">
         <v>4916760481.71637</v>
       </c>
-      <c r="AL25" s="5" t="n">
+      <c r="AL25" s="10" t="n">
         <v>877073688.397079</v>
       </c>
-      <c r="AM25" s="5" t="n">
+      <c r="AM25" s="10" t="n">
         <v>1039083214.83595</v>
       </c>
-      <c r="AN25" s="5" t="n">
+      <c r="AN25" s="10" t="n">
         <v>890083254.945149</v>
       </c>
-      <c r="AO25" s="5" t="n">
+      <c r="AO25" s="10" t="n">
         <v>902878503.120584</v>
       </c>
-      <c r="AP25" s="5" t="n">
+      <c r="AP25" s="10" t="n">
         <v>1397886258.68569</v>
       </c>
-      <c r="AQ25" s="5" t="n">
+      <c r="AQ25" s="10" t="n">
         <v>24128.2435797438</v>
       </c>
-      <c r="AR25" s="5" t="n">
+      <c r="AR25" s="10" t="n">
         <v>59684.9236466806</v>
       </c>
-      <c r="AS25" s="5" t="n">
+      <c r="AS25" s="10" t="n">
         <v>11573.9072704938</v>
       </c>
-      <c r="AT25" s="5" t="n">
+      <c r="AT25" s="10" t="n">
         <v>11188.817598517</v>
       </c>
-      <c r="AU25" s="5" t="n">
+      <c r="AU25" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="AV25" s="5" t="n">
+      <c r="AV25" s="10" t="n">
         <v>-29324.9492</v>
       </c>
-      <c r="AW25" s="5" t="n">
+      <c r="AW25" s="10" t="n">
         <v>9739.88670259903</v>
       </c>
-      <c r="AX25" s="5"/>
+      <c r="AX25" s="10"/>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -5775,16 +5775,16 @@
       <c r="B26" t="str">
         <f>N26</f>
       </c>
-      <c r="C26" s="5" t="str">
+      <c r="C26" s="10" t="str">
         <f>AS26</f>
       </c>
-      <c r="D26" s="5" t="str">
+      <c r="D26" s="10" t="str">
         <f>AV26</f>
       </c>
-      <c r="E26" s="5" t="str">
+      <c r="E26" s="10" t="str">
         <f>AW26</f>
       </c>
-      <c r="F26" s="5" t="str">
+      <c r="F26" s="10" t="str">
         <f>AX26</f>
       </c>
       <c r="G26" s="2" t="str">
@@ -5808,112 +5808,112 @@
       <c r="N26" t="s">
         <v>21</v>
       </c>
-      <c r="O26" s="5" t="str">
+      <c r="O26" s="10" t="str">
         <f>Sum(O16:O25)</f>
       </c>
-      <c r="P26" s="5" t="str">
+      <c r="P26" s="10" t="str">
         <f>Sum(P16:P25)</f>
       </c>
-      <c r="Q26" s="5" t="str">
+      <c r="Q26" s="10" t="str">
         <f>Sum(Q16:Q25)</f>
       </c>
-      <c r="R26" s="5" t="str">
+      <c r="R26" s="10" t="str">
         <f>Sum(R16:R25)</f>
       </c>
-      <c r="S26" s="5" t="str">
+      <c r="S26" s="10" t="str">
         <f>Sum(S16:S25)</f>
       </c>
-      <c r="T26" s="5" t="str">
+      <c r="T26" s="10" t="str">
         <f>Sum(T16:T25)</f>
       </c>
-      <c r="U26" s="5" t="str">
+      <c r="U26" s="10" t="str">
         <f>Sum(U16:U25)</f>
       </c>
-      <c r="V26" s="5" t="str">
+      <c r="V26" s="10" t="str">
         <f>Sum(V16:V25)</f>
       </c>
-      <c r="W26" s="5" t="str">
+      <c r="W26" s="10" t="str">
         <f>Sum(W16:W25)</f>
       </c>
-      <c r="X26" s="5" t="str">
+      <c r="X26" s="10" t="str">
         <f>Sum(X16:X25)</f>
       </c>
-      <c r="Y26" s="5" t="str">
+      <c r="Y26" s="10" t="str">
         <f>Sum(Y16:Y25)</f>
       </c>
-      <c r="Z26" s="5" t="str">
+      <c r="Z26" s="10" t="str">
         <f>Sum(Z16:Z25)</f>
       </c>
-      <c r="AA26" s="5" t="str">
+      <c r="AA26" s="10" t="str">
         <f>Sum(AA16:AA25)</f>
       </c>
-      <c r="AB26" s="5" t="str">
+      <c r="AB26" s="10" t="str">
         <f>Sum(AB16:AB25)</f>
       </c>
-      <c r="AC26" s="5" t="str">
+      <c r="AC26" s="10" t="str">
         <f>Sum(AC16:AC25)</f>
       </c>
-      <c r="AD26" s="5" t="str">
+      <c r="AD26" s="10" t="str">
         <f>Sum(AD16:AD25)</f>
       </c>
-      <c r="AE26" s="5" t="str">
+      <c r="AE26" s="10" t="str">
         <f>Sum(AE16:AE25)</f>
       </c>
-      <c r="AF26" s="5" t="str">
+      <c r="AF26" s="10" t="str">
         <f>Sum(AF16:AF25)</f>
       </c>
-      <c r="AG26" s="5" t="str">
+      <c r="AG26" s="10" t="str">
         <f>Sum(AG16:AG25)</f>
       </c>
-      <c r="AH26" s="5" t="str">
+      <c r="AH26" s="10" t="str">
         <f>Sum(AH16:AH25)</f>
       </c>
-      <c r="AI26" s="5" t="str">
+      <c r="AI26" s="10" t="str">
         <f>Sum(AI16:AI25)</f>
       </c>
-      <c r="AJ26" s="5" t="str">
+      <c r="AJ26" s="10" t="str">
         <f>Sum(AJ16:AJ25)</f>
       </c>
-      <c r="AK26" s="5" t="str">
+      <c r="AK26" s="10" t="str">
         <f>Sum(AK16:AK25)</f>
       </c>
-      <c r="AL26" s="5" t="str">
+      <c r="AL26" s="10" t="str">
         <f>Sum(AL16:AL25)</f>
       </c>
-      <c r="AM26" s="5" t="str">
+      <c r="AM26" s="10" t="str">
         <f>Sum(AM16:AM25)</f>
       </c>
-      <c r="AN26" s="5" t="str">
+      <c r="AN26" s="10" t="str">
         <f>Sum(AN16:AN25)</f>
       </c>
-      <c r="AO26" s="5" t="str">
+      <c r="AO26" s="10" t="str">
         <f>Sum(AO16:AO25)</f>
       </c>
-      <c r="AP26" s="5" t="str">
+      <c r="AP26" s="10" t="str">
         <f>Sum(AP16:AP25)</f>
       </c>
-      <c r="AQ26" s="5" t="str">
+      <c r="AQ26" s="10" t="str">
         <f>Sum(AQ16:AQ25)</f>
       </c>
-      <c r="AR26" s="5" t="str">
+      <c r="AR26" s="10" t="str">
         <f>Sum(AR16:AR25)</f>
       </c>
-      <c r="AS26" s="5" t="str">
+      <c r="AS26" s="10" t="str">
         <f>Sum(AS16:AS25)</f>
       </c>
-      <c r="AT26" s="5" t="str">
+      <c r="AT26" s="10" t="str">
         <f>Sum(AT16:AT25)</f>
       </c>
-      <c r="AU26" s="5" t="str">
+      <c r="AU26" s="10" t="str">
         <f>Sum(AU16:AU25)</f>
       </c>
-      <c r="AV26" s="5" t="str">
+      <c r="AV26" s="10" t="str">
         <f>Sum(AV16:AV25)</f>
       </c>
-      <c r="AW26" s="5" t="str">
+      <c r="AW26" s="10" t="str">
         <f>Sum(AW16:AW25)</f>
       </c>
-      <c r="AX26" s="5"/>
+      <c r="AX26" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21925,83 +21925,83 @@
       <c r="L2" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="10" t="n">
+      <c r="M2" s="9" t="n">
         <v>6381928579.3536</v>
       </c>
-      <c r="N2" s="10" t="n">
+      <c r="N2" s="9" t="n">
         <v>6747108088.619</v>
       </c>
-      <c r="O2" s="10" t="n">
+      <c r="O2" s="9" t="n">
         <v>8072281192.2013</v>
       </c>
-      <c r="P2" s="10" t="n">
+      <c r="P2" s="9" t="n">
         <v>10540757674.2942</v>
       </c>
-      <c r="Q2" s="10" t="n">
+      <c r="Q2" s="9" t="n">
         <v>12837555957.1638</v>
       </c>
-      <c r="R2" s="10" t="n">
+      <c r="R2" s="9" t="n">
         <v>15096204296.5031</v>
       </c>
-      <c r="S2" s="10" t="n">
+      <c r="S2" s="9" t="n">
         <v>20557893154.9814</v>
       </c>
-      <c r="T2" s="10" t="n">
+      <c r="T2" s="9" t="n">
         <v>37399824102.3718</v>
       </c>
-      <c r="U2" s="10" t="n">
+      <c r="U2" s="9" t="n">
         <v>49726656794.9868</v>
       </c>
-      <c r="V2" s="10" t="n">
+      <c r="V2" s="9" t="n">
         <v>54631556718.4632</v>
       </c>
-      <c r="W2" s="10" t="n">
+      <c r="W2" s="9" t="n">
         <v>18690465759.476</v>
       </c>
-      <c r="X2" s="10" t="n">
+      <c r="X2" s="9" t="n">
         <v>13792564390.7305</v>
       </c>
-      <c r="Y2" s="10" t="n">
+      <c r="Y2" s="9" t="n">
         <v>9960146812.9704</v>
       </c>
-      <c r="Z2" s="10" t="n">
+      <c r="Z2" s="9" t="n">
         <v>5674820889.0681</v>
       </c>
-      <c r="AA2" s="10" t="n">
+      <c r="AA2" s="9" t="n">
         <v>3560661708.8258</v>
       </c>
-      <c r="AB2" s="10" t="n">
+      <c r="AB2" s="9" t="n">
         <v>3309138661.2531</v>
       </c>
-      <c r="AC2" s="10" t="n">
+      <c r="AC2" s="9" t="n">
         <v>3497892252.0064</v>
       </c>
-      <c r="AD2" s="10" t="n">
+      <c r="AD2" s="9" t="n">
         <v>3785717114.4289</v>
       </c>
-      <c r="AE2" s="10" t="n">
+      <c r="AE2" s="9" t="n">
         <v>5065767840.963</v>
       </c>
-      <c r="AF2" s="10" t="n">
+      <c r="AF2" s="9" t="n">
         <v>5080092983.2125</v>
       </c>
-      <c r="AG2" s="10" t="n">
+      <c r="AG2" s="9" t="n">
         <v>5492573941.4207</v>
       </c>
-      <c r="AH2" s="10" t="n">
+      <c r="AH2" s="9" t="n">
         <v>5019427737.2304</v>
       </c>
-      <c r="AI2" s="10" t="n">
+      <c r="AI2" s="9" t="n">
         <v>4855696567.4635</v>
       </c>
-      <c r="AJ2" s="10" t="n">
+      <c r="AJ2" s="9" t="n">
         <v>6240783323.4101</v>
       </c>
-      <c r="AK2" s="10" t="n">
+      <c r="AK2" s="9" t="n">
         <v>7219861841.72</v>
       </c>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -22010,83 +22010,83 @@
       <c r="L3" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="10" t="n">
+      <c r="M3" s="9" t="n">
         <v>41017731029.8018</v>
       </c>
-      <c r="N3" s="10" t="n">
+      <c r="N3" s="9" t="n">
         <v>43077261719.4941</v>
       </c>
-      <c r="O3" s="10" t="n">
+      <c r="O3" s="9" t="n">
         <v>47986493060.5011</v>
       </c>
-      <c r="P3" s="10" t="n">
+      <c r="P3" s="9" t="n">
         <v>60359498534.808</v>
       </c>
-      <c r="Q3" s="10" t="n">
+      <c r="Q3" s="9" t="n">
         <v>72636344256.3692</v>
       </c>
-      <c r="R3" s="10" t="n">
+      <c r="R3" s="9" t="n">
         <v>78922436134.7553</v>
       </c>
-      <c r="S3" s="10" t="n">
+      <c r="S3" s="9" t="n">
         <v>91529553402.1407</v>
       </c>
-      <c r="T3" s="10" t="n">
+      <c r="T3" s="9" t="n">
         <v>90597609774.4867</v>
       </c>
-      <c r="U3" s="10" t="n">
+      <c r="U3" s="9" t="n">
         <v>92243967300.8319</v>
       </c>
-      <c r="V3" s="10" t="n">
+      <c r="V3" s="9" t="n">
         <v>93384043495.1289</v>
       </c>
-      <c r="W3" s="10" t="n">
+      <c r="W3" s="9" t="n">
         <v>106597055566.163</v>
       </c>
-      <c r="X3" s="10" t="n">
+      <c r="X3" s="9" t="n">
         <v>114593342600.983</v>
       </c>
-      <c r="Y3" s="10" t="n">
+      <c r="Y3" s="9" t="n">
         <v>101983846618.247</v>
       </c>
-      <c r="Z3" s="10" t="n">
+      <c r="Z3" s="9" t="n">
         <v>95556972800.1595</v>
       </c>
-      <c r="AA3" s="10" t="n">
+      <c r="AA3" s="9" t="n">
         <v>92928871336.1869</v>
       </c>
-      <c r="AB3" s="10" t="n">
+      <c r="AB3" s="9" t="n">
         <v>88179253906.2632</v>
       </c>
-      <c r="AC3" s="10" t="n">
+      <c r="AC3" s="9" t="n">
         <v>91924227580.0939</v>
       </c>
-      <c r="AD3" s="10" t="n">
+      <c r="AD3" s="9" t="n">
         <v>98723360346.6838</v>
       </c>
-      <c r="AE3" s="10" t="n">
+      <c r="AE3" s="9" t="n">
         <v>101053858127.361</v>
       </c>
-      <c r="AF3" s="10" t="n">
+      <c r="AF3" s="9" t="n">
         <v>108597077492.154</v>
       </c>
-      <c r="AG3" s="10" t="n">
+      <c r="AG3" s="9" t="n">
         <v>108114538828.644</v>
       </c>
-      <c r="AH3" s="10" t="n">
+      <c r="AH3" s="9" t="n">
         <v>113102366189.102</v>
       </c>
-      <c r="AI3" s="10" t="n">
+      <c r="AI3" s="9" t="n">
         <v>118414679206.352</v>
       </c>
-      <c r="AJ3" s="10" t="n">
+      <c r="AJ3" s="9" t="n">
         <v>127278745636.945</v>
       </c>
-      <c r="AK3" s="10" t="n">
+      <c r="AK3" s="9" t="n">
         <v>140190170596.9</v>
       </c>
-      <c r="AL3" s="10"/>
-      <c r="AM3" s="10"/>
+      <c r="AL3" s="9"/>
+      <c r="AM3" s="9"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -22095,83 +22095,83 @@
       <c r="L4" t="s">
         <v>55</v>
       </c>
-      <c r="M4" s="10" t="n">
+      <c r="M4" s="9" t="n">
         <v>65729849056.083</v>
       </c>
-      <c r="N4" s="10" t="n">
+      <c r="N4" s="9" t="n">
         <v>73056891006.8772</v>
       </c>
-      <c r="O4" s="10" t="n">
+      <c r="O4" s="9" t="n">
         <v>87658370256.8362</v>
       </c>
-      <c r="P4" s="10" t="n">
+      <c r="P4" s="9" t="n">
         <v>112233600483.614</v>
       </c>
-      <c r="Q4" s="10" t="n">
+      <c r="Q4" s="9" t="n">
         <v>113809654964.141</v>
       </c>
-      <c r="R4" s="10" t="n">
+      <c r="R4" s="9" t="n">
         <v>135269794700.926</v>
       </c>
-      <c r="S4" s="10" t="n">
+      <c r="S4" s="9" t="n">
         <v>151371749273.841</v>
       </c>
-      <c r="T4" s="10" t="n">
+      <c r="T4" s="9" t="n">
         <v>176305123926.349</v>
       </c>
-      <c r="U4" s="10" t="n">
+      <c r="U4" s="9" t="n">
         <v>201282666535.121</v>
       </c>
-      <c r="V4" s="10" t="n">
+      <c r="V4" s="9" t="n">
         <v>182260902974.079</v>
       </c>
-      <c r="W4" s="10" t="n">
+      <c r="W4" s="9" t="n">
         <v>205091243389.123</v>
       </c>
-      <c r="X4" s="10" t="n">
+      <c r="X4" s="9" t="n">
         <v>196042614484.438</v>
       </c>
-      <c r="Y4" s="10" t="n">
+      <c r="Y4" s="9" t="n">
         <v>190911668190.224</v>
       </c>
-      <c r="Z4" s="10" t="n">
+      <c r="Z4" s="9" t="n">
         <v>154549244061.639</v>
       </c>
-      <c r="AA4" s="10" t="n">
+      <c r="AA4" s="9" t="n">
         <v>150023467175.449</v>
       </c>
-      <c r="AB4" s="10" t="n">
+      <c r="AB4" s="9" t="n">
         <v>148167793539.232</v>
       </c>
-      <c r="AC4" s="10" t="n">
+      <c r="AC4" s="9" t="n">
         <v>162671372686.458</v>
       </c>
-      <c r="AD4" s="10" t="n">
+      <c r="AD4" s="9" t="n">
         <v>164423899394.237</v>
       </c>
-      <c r="AE4" s="10" t="n">
+      <c r="AE4" s="9" t="n">
         <v>186214236769.723</v>
       </c>
-      <c r="AF4" s="10" t="n">
+      <c r="AF4" s="9" t="n">
         <v>202877106832.583</v>
       </c>
-      <c r="AG4" s="10" t="n">
+      <c r="AG4" s="9" t="n">
         <v>223388717765.705</v>
       </c>
-      <c r="AH4" s="10" t="n">
+      <c r="AH4" s="9" t="n">
         <v>221867314116.506</v>
       </c>
-      <c r="AI4" s="10" t="n">
+      <c r="AI4" s="9" t="n">
         <v>229190166357.694</v>
       </c>
-      <c r="AJ4" s="10" t="n">
+      <c r="AJ4" s="9" t="n">
         <v>241088412575.15</v>
       </c>
-      <c r="AK4" s="10" t="n">
+      <c r="AK4" s="9" t="n">
         <v>241348214838.25</v>
       </c>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="9"/>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -22180,83 +22180,83 @@
       <c r="L5" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="10" t="n">
+      <c r="M5" s="9" t="n">
         <v>6301955255</v>
       </c>
-      <c r="N5" s="10" t="n">
+      <c r="N5" s="9" t="n">
         <v>8495776002</v>
       </c>
-      <c r="O5" s="10" t="n">
+      <c r="O5" s="9" t="n">
         <v>8579162029</v>
       </c>
-      <c r="P5" s="10" t="n">
+      <c r="P5" s="9" t="n">
         <v>10237410913.1396</v>
       </c>
-      <c r="Q5" s="10" t="n">
+      <c r="Q5" s="9" t="n">
         <v>11393769098.2552</v>
       </c>
-      <c r="R5" s="10" t="n">
+      <c r="R5" s="9" t="n">
         <v>22121395381.4164</v>
       </c>
-      <c r="S5" s="10" t="n">
+      <c r="S5" s="9" t="n">
         <v>19911512736.7794</v>
       </c>
-      <c r="T5" s="10" t="n">
+      <c r="T5" s="9" t="n">
         <v>17480281868.3767</v>
       </c>
-      <c r="U5" s="10" t="n">
+      <c r="U5" s="9" t="n">
         <v>23192843019.3978</v>
       </c>
-      <c r="V5" s="10" t="n">
+      <c r="V5" s="9" t="n">
         <v>24772255556.7469</v>
       </c>
-      <c r="W5" s="10" t="n">
+      <c r="W5" s="9" t="n">
         <v>17167106144.1264</v>
       </c>
-      <c r="X5" s="10" t="n">
+      <c r="X5" s="9" t="n">
         <v>19616156026.3993</v>
       </c>
-      <c r="Y5" s="10" t="n">
+      <c r="Y5" s="9" t="n">
         <v>27118150470.6684</v>
       </c>
-      <c r="Z5" s="10" t="n">
+      <c r="Z5" s="9" t="n">
         <v>18300928885.4694</v>
       </c>
-      <c r="AA5" s="10" t="n">
+      <c r="AA5" s="9" t="n">
         <v>11867343341.3143</v>
       </c>
-      <c r="AB5" s="10" t="n">
+      <c r="AB5" s="9" t="n">
         <v>8985851310.0384</v>
       </c>
-      <c r="AC5" s="10" t="n">
+      <c r="AC5" s="9" t="n">
         <v>7381526904.9523</v>
       </c>
-      <c r="AD5" s="10" t="n">
+      <c r="AD5" s="9" t="n">
         <v>9214656305.5226</v>
       </c>
-      <c r="AE5" s="10" t="n">
+      <c r="AE5" s="9" t="n">
         <v>10630900917.601</v>
       </c>
-      <c r="AF5" s="10" t="n">
+      <c r="AF5" s="9" t="n">
         <v>9804333730.5025</v>
       </c>
-      <c r="AG5" s="10" t="n">
+      <c r="AG5" s="9" t="n">
         <v>8945182432.6572</v>
       </c>
-      <c r="AH5" s="10" t="n">
+      <c r="AH5" s="9" t="n">
         <v>10400372579.0701</v>
       </c>
-      <c r="AI5" s="10" t="n">
+      <c r="AI5" s="9" t="n">
         <v>17547545516.7689</v>
       </c>
-      <c r="AJ5" s="10" t="n">
+      <c r="AJ5" s="9" t="n">
         <v>16981868245.7354</v>
       </c>
-      <c r="AK5" s="10" t="n">
+      <c r="AK5" s="9" t="n">
         <v>17457190518.18</v>
       </c>
-      <c r="AL5" s="10"/>
-      <c r="AM5" s="10"/>
+      <c r="AL5" s="9"/>
+      <c r="AM5" s="9"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -22265,166 +22265,166 @@
       <c r="L6" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="10" t="n">
+      <c r="M6" s="9" t="n">
         <v>6133098636</v>
       </c>
-      <c r="N6" s="10" t="n">
+      <c r="N6" s="9" t="n">
         <v>6192593184</v>
       </c>
-      <c r="O6" s="10" t="n">
+      <c r="O6" s="9" t="n">
         <v>9031564886</v>
       </c>
-      <c r="P6" s="10" t="n">
+      <c r="P6" s="9" t="n">
         <v>9079232479</v>
       </c>
-      <c r="Q6" s="10" t="n">
+      <c r="Q6" s="9" t="n">
         <v>9827511407.49</v>
       </c>
-      <c r="R6" s="10" t="n">
+      <c r="R6" s="9" t="n">
         <v>6844005103.9382</v>
       </c>
-      <c r="S6" s="10" t="n">
+      <c r="S6" s="9" t="n">
         <v>7082066073.0875</v>
       </c>
-      <c r="T6" s="10" t="n">
+      <c r="T6" s="9" t="n">
         <v>5551385159.2825</v>
       </c>
-      <c r="U6" s="10" t="n">
+      <c r="U6" s="9" t="n">
         <v>5349736696.5096</v>
       </c>
-      <c r="V6" s="10" t="n">
+      <c r="V6" s="9" t="n">
         <v>9307112508.7261</v>
       </c>
-      <c r="W6" s="10" t="n">
+      <c r="W6" s="9" t="n">
         <v>14936091789.0248</v>
       </c>
-      <c r="X6" s="10" t="n">
+      <c r="X6" s="9" t="n">
         <v>24522062766.4876</v>
       </c>
-      <c r="Y6" s="10" t="n">
+      <c r="Y6" s="9" t="n">
         <v>27821465995.2082</v>
       </c>
-      <c r="Z6" s="10" t="n">
+      <c r="Z6" s="9" t="n">
         <v>34145937904.3437</v>
       </c>
-      <c r="AA6" s="10" t="n">
+      <c r="AA6" s="9" t="n">
         <v>25072028857.0941</v>
       </c>
-      <c r="AB6" s="10" t="n">
+      <c r="AB6" s="9" t="n">
         <v>25584172858.1798</v>
       </c>
-      <c r="AC6" s="10" t="n">
+      <c r="AC6" s="9" t="n">
         <v>33049812670.3039</v>
       </c>
-      <c r="AD6" s="10" t="n">
+      <c r="AD6" s="9" t="n">
         <v>45706086881.0323</v>
       </c>
-      <c r="AE6" s="10" t="n">
+      <c r="AE6" s="9" t="n">
         <v>55865325274.4157</v>
       </c>
-      <c r="AF6" s="10" t="n">
+      <c r="AF6" s="9" t="n">
         <v>57616963401.306</v>
       </c>
-      <c r="AG6" s="10" t="n">
+      <c r="AG6" s="9" t="n">
         <v>76806621768.5092</v>
       </c>
-      <c r="AH6" s="10" t="n">
+      <c r="AH6" s="9" t="n">
         <v>37313582245.916</v>
       </c>
-      <c r="AI6" s="10" t="n">
+      <c r="AI6" s="9" t="n">
         <v>44487852773.861</v>
       </c>
-      <c r="AJ6" s="10" t="n">
+      <c r="AJ6" s="9" t="n">
         <v>64656951414.6669</v>
       </c>
-      <c r="AK6" s="10" t="n">
+      <c r="AK6" s="9" t="n">
         <v>38828429967.57</v>
       </c>
-      <c r="AL6" s="10"/>
-      <c r="AM6" s="10"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <f>L7</f>
       </c>
       <c r="L7"/>
-      <c r="M7" s="10" t="n">
+      <c r="M7" s="9" t="n">
         <v>6613923950.149</v>
       </c>
-      <c r="N7" s="10" t="n">
+      <c r="N7" s="9" t="n">
         <v>6424008621.3371</v>
       </c>
-      <c r="O7" s="10" t="n">
+      <c r="O7" s="9" t="n">
         <v>8482649711.9464</v>
       </c>
-      <c r="P7" s="10" t="n">
+      <c r="P7" s="9" t="n">
         <v>9082587219.0046</v>
       </c>
-      <c r="Q7" s="10" t="n">
+      <c r="Q7" s="9" t="n">
         <v>9270196138.4963</v>
       </c>
-      <c r="R7" s="10" t="n">
+      <c r="R7" s="9" t="n">
         <v>7410683084.917</v>
       </c>
-      <c r="S7" s="10" t="n">
+      <c r="S7" s="9" t="n">
         <v>4712411702.288</v>
       </c>
-      <c r="T7" s="10" t="n">
+      <c r="T7" s="9" t="n">
         <v>820198022.6251</v>
       </c>
-      <c r="U7" s="10" t="n">
+      <c r="U7" s="9" t="n">
         <v>6192215737.982</v>
       </c>
-      <c r="V7" s="10" t="n">
+      <c r="V7" s="9" t="n">
         <v>3294194225.2823</v>
       </c>
-      <c r="W7" s="10" t="n">
+      <c r="W7" s="9" t="n">
         <v>214382588.7513</v>
       </c>
-      <c r="X7" s="10" t="n">
+      <c r="X7" s="9" t="n">
         <v>-3081399.5465</v>
       </c>
-      <c r="Y7" s="10" t="n">
+      <c r="Y7" s="9" t="n">
         <v>-1973038.6911</v>
       </c>
-      <c r="Z7" s="10" t="n">
+      <c r="Z7" s="9" t="n">
         <v>508721.45</v>
       </c>
-      <c r="AA7" s="10" t="n">
+      <c r="AA7" s="9" t="n">
         <v>-2834591.3209</v>
       </c>
-      <c r="AB7" s="10" t="n">
+      <c r="AB7" s="9" t="n">
         <v>29995.58</v>
       </c>
-      <c r="AC7" s="10" t="n">
+      <c r="AC7" s="9" t="n">
         <v>-58489.62</v>
       </c>
-      <c r="AD7" s="10" t="n">
+      <c r="AD7" s="9" t="n">
         <v>1356734.2</v>
       </c>
-      <c r="AE7" s="10" t="n">
+      <c r="AE7" s="9" t="n">
         <v>20204.7109</v>
       </c>
-      <c r="AF7" s="10" t="n">
+      <c r="AF7" s="9" t="n">
         <v>50903.5586</v>
       </c>
-      <c r="AG7" s="10" t="n">
+      <c r="AG7" s="9" t="n">
         <v>10000</v>
       </c>
-      <c r="AH7" s="10" t="n">
+      <c r="AH7" s="9" t="n">
         <v>10000</v>
       </c>
-      <c r="AI7" s="10" t="n">
+      <c r="AI7" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="AJ7" s="10" t="n">
+      <c r="AJ7" s="9" t="n">
         <v>-29324.9492</v>
       </c>
-      <c r="AK7" s="10" t="n">
+      <c r="AK7" s="9" t="n">
         <v>10000</v>
       </c>
-      <c r="AL7" s="10"/>
-      <c r="AM7" s="10"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -22433,85 +22433,85 @@
       <c r="L8" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="10" t="str">
+      <c r="M8" s="9" t="str">
         <f>Sum(M2:M7)</f>
       </c>
-      <c r="N8" s="10" t="str">
+      <c r="N8" s="9" t="str">
         <f>Sum(N2:N7)</f>
       </c>
-      <c r="O8" s="10" t="str">
+      <c r="O8" s="9" t="str">
         <f>Sum(O2:O7)</f>
       </c>
-      <c r="P8" s="10" t="str">
+      <c r="P8" s="9" t="str">
         <f>Sum(P2:P7)</f>
       </c>
-      <c r="Q8" s="10" t="str">
+      <c r="Q8" s="9" t="str">
         <f>Sum(Q2:Q7)</f>
       </c>
-      <c r="R8" s="10" t="str">
+      <c r="R8" s="9" t="str">
         <f>Sum(R2:R7)</f>
       </c>
-      <c r="S8" s="10" t="str">
+      <c r="S8" s="9" t="str">
         <f>Sum(S2:S7)</f>
       </c>
-      <c r="T8" s="10" t="str">
+      <c r="T8" s="9" t="str">
         <f>Sum(T2:T7)</f>
       </c>
-      <c r="U8" s="10" t="str">
+      <c r="U8" s="9" t="str">
         <f>Sum(U2:U7)</f>
       </c>
-      <c r="V8" s="10" t="str">
+      <c r="V8" s="9" t="str">
         <f>Sum(V2:V7)</f>
       </c>
-      <c r="W8" s="10" t="str">
+      <c r="W8" s="9" t="str">
         <f>Sum(W2:W7)</f>
       </c>
-      <c r="X8" s="10" t="str">
+      <c r="X8" s="9" t="str">
         <f>Sum(X2:X7)</f>
       </c>
-      <c r="Y8" s="10" t="str">
+      <c r="Y8" s="9" t="str">
         <f>Sum(Y2:Y7)</f>
       </c>
-      <c r="Z8" s="10" t="str">
+      <c r="Z8" s="9" t="str">
         <f>Sum(Z2:Z7)</f>
       </c>
-      <c r="AA8" s="10" t="str">
+      <c r="AA8" s="9" t="str">
         <f>Sum(AA2:AA7)</f>
       </c>
-      <c r="AB8" s="10" t="str">
+      <c r="AB8" s="9" t="str">
         <f>Sum(AB2:AB7)</f>
       </c>
-      <c r="AC8" s="10" t="str">
+      <c r="AC8" s="9" t="str">
         <f>Sum(AC2:AC7)</f>
       </c>
-      <c r="AD8" s="10" t="str">
+      <c r="AD8" s="9" t="str">
         <f>Sum(AD2:AD7)</f>
       </c>
-      <c r="AE8" s="10" t="str">
+      <c r="AE8" s="9" t="str">
         <f>Sum(AE2:AE7)</f>
       </c>
-      <c r="AF8" s="10" t="str">
+      <c r="AF8" s="9" t="str">
         <f>Sum(AF2:AF7)</f>
       </c>
-      <c r="AG8" s="10" t="str">
+      <c r="AG8" s="9" t="str">
         <f>Sum(AG2:AG7)</f>
       </c>
-      <c r="AH8" s="10" t="str">
+      <c r="AH8" s="9" t="str">
         <f>Sum(AH2:AH7)</f>
       </c>
-      <c r="AI8" s="10" t="str">
+      <c r="AI8" s="9" t="str">
         <f>Sum(AI2:AI7)</f>
       </c>
-      <c r="AJ8" s="10" t="str">
+      <c r="AJ8" s="9" t="str">
         <f>Sum(AJ2:AJ7)</f>
       </c>
-      <c r="AK8" s="10" t="str">
+      <c r="AK8" s="9" t="str">
         <f>Sum(AK2:AK7)</f>
       </c>
-      <c r="AL8" s="10" t="str">
+      <c r="AL8" s="9" t="str">
         <f>Sum(AL2:AL7)</f>
       </c>
-      <c r="AM8" s="10"/>
+      <c r="AM8" s="9"/>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -22618,16 +22618,16 @@
       <c r="A12" t="str">
         <f>L12</f>
       </c>
-      <c r="B12" s="10" t="str">
+      <c r="B12" s="9" t="str">
         <f>AG12</f>
       </c>
-      <c r="C12" s="10" t="str">
+      <c r="C12" s="9" t="str">
         <f>AJ12</f>
       </c>
-      <c r="D12" s="10" t="str">
+      <c r="D12" s="9" t="str">
         <f>AK12</f>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="2" t="str">
         <f>AK12/AJ12-1</f>
       </c>
@@ -22642,98 +22642,98 @@
       <c r="L12" t="s">
         <v>69</v>
       </c>
-      <c r="M12" s="10" t="n">
+      <c r="M12" s="9" t="n">
         <v>10729128513.2762</v>
       </c>
-      <c r="N12" s="10" t="n">
+      <c r="N12" s="9" t="n">
         <v>11074619926.2147</v>
       </c>
-      <c r="O12" s="10" t="n">
+      <c r="O12" s="9" t="n">
         <v>13044524297.5751</v>
       </c>
-      <c r="P12" s="10" t="n">
+      <c r="P12" s="9" t="n">
         <v>16712693706.8193</v>
       </c>
-      <c r="Q12" s="10" t="n">
+      <c r="Q12" s="9" t="n">
         <v>19869157547.3429</v>
       </c>
-      <c r="R12" s="10" t="n">
+      <c r="R12" s="9" t="n">
         <v>22674955819.7369</v>
       </c>
-      <c r="S12" s="10" t="n">
+      <c r="S12" s="9" t="n">
         <v>29907067291.4277</v>
       </c>
-      <c r="T12" s="10" t="n">
+      <c r="T12" s="9" t="n">
         <v>52950551255.7345</v>
       </c>
-      <c r="U12" s="10" t="n">
+      <c r="U12" s="9" t="n">
         <v>68970946398.2195</v>
       </c>
-      <c r="V12" s="10" t="n">
+      <c r="V12" s="9" t="n">
         <v>75007019736.8259</v>
       </c>
-      <c r="W12" s="10" t="n">
+      <c r="W12" s="9" t="n">
         <v>25440958456.9914</v>
       </c>
-      <c r="X12" s="10" t="n">
+      <c r="X12" s="9" t="n">
         <v>18404660431.2842</v>
       </c>
-      <c r="Y12" s="10" t="n">
+      <c r="Y12" s="9" t="n">
         <v>13053844985.2393</v>
       </c>
-      <c r="Z12" s="10" t="n">
+      <c r="Z12" s="9" t="n">
         <v>7304918123.92328</v>
       </c>
-      <c r="AA12" s="10" t="n">
+      <c r="AA12" s="9" t="n">
         <v>4501346052.24413</v>
       </c>
-      <c r="AB12" s="10" t="n">
+      <c r="AB12" s="9" t="n">
         <v>4140493607.75378</v>
       </c>
-      <c r="AC12" s="10" t="n">
+      <c r="AC12" s="9" t="n">
         <v>4341953501.98336</v>
       </c>
-      <c r="AD12" s="10" t="n">
+      <c r="AD12" s="9" t="n">
         <v>4621224882.4711</v>
       </c>
-      <c r="AE12" s="10" t="n">
+      <c r="AE12" s="9" t="n">
         <v>6049484250.98168</v>
       </c>
-      <c r="AF12" s="10" t="n">
+      <c r="AF12" s="9" t="n">
         <v>5956459040.5881</v>
       </c>
-      <c r="AG12" s="10" t="n">
+      <c r="AG12" s="9" t="n">
         <v>6357054147.4334</v>
       </c>
-      <c r="AH12" s="10" t="n">
+      <c r="AH12" s="9" t="n">
         <v>5616146140.08081</v>
       </c>
-      <c r="AI12" s="10" t="n">
+      <c r="AI12" s="9" t="n">
         <v>5077828150.4119</v>
       </c>
-      <c r="AJ12" s="10" t="n">
+      <c r="AJ12" s="9" t="n">
         <v>6240783323.4101</v>
       </c>
-      <c r="AK12" s="10" t="n">
+      <c r="AK12" s="9" t="n">
         <v>7032063634.67708</v>
       </c>
-      <c r="AL12" s="10"/>
-      <c r="AM12" s="10"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
     </row>
     <row r="13">
       <c r="A13" t="str">
         <f>L13</f>
       </c>
-      <c r="B13" s="10" t="str">
+      <c r="B13" s="9" t="str">
         <f>AG13</f>
       </c>
-      <c r="C13" s="10" t="str">
+      <c r="C13" s="9" t="str">
         <f>AJ13</f>
       </c>
-      <c r="D13" s="10" t="str">
+      <c r="D13" s="9" t="str">
         <f>AK13</f>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="2" t="str">
         <f>AK13/AJ13-1</f>
       </c>
@@ -22748,98 +22748,98 @@
       <c r="L13" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="10" t="n">
+      <c r="M13" s="9" t="n">
         <v>68957917981.9518</v>
       </c>
-      <c r="N13" s="10" t="n">
+      <c r="N13" s="9" t="n">
         <v>70706485614.2123</v>
       </c>
-      <c r="O13" s="10" t="n">
+      <c r="O13" s="9" t="n">
         <v>77544495760.1167</v>
       </c>
-      <c r="P13" s="10" t="n">
+      <c r="P13" s="9" t="n">
         <v>95701831166.2309</v>
       </c>
-      <c r="Q13" s="10" t="n">
+      <c r="Q13" s="9" t="n">
         <v>112421941723.843</v>
       </c>
-      <c r="R13" s="10" t="n">
+      <c r="R13" s="9" t="n">
         <v>118543888078.947</v>
       </c>
-      <c r="S13" s="10" t="n">
+      <c r="S13" s="9" t="n">
         <v>133154720287.514</v>
       </c>
-      <c r="T13" s="10" t="n">
+      <c r="T13" s="9" t="n">
         <v>128267805936.199</v>
       </c>
-      <c r="U13" s="10" t="n">
+      <c r="U13" s="9" t="n">
         <v>127942518848.486</v>
       </c>
-      <c r="V13" s="10" t="n">
+      <c r="V13" s="9" t="n">
         <v>128212689044.179</v>
       </c>
-      <c r="W13" s="10" t="n">
+      <c r="W13" s="9" t="n">
         <v>145097040234.079</v>
       </c>
-      <c r="X13" s="10" t="n">
+      <c r="X13" s="9" t="n">
         <v>152912214038.626</v>
       </c>
-      <c r="Y13" s="10" t="n">
+      <c r="Y13" s="9" t="n">
         <v>133660813414.857</v>
       </c>
-      <c r="Z13" s="10" t="n">
+      <c r="Z13" s="9" t="n">
         <v>123005796327.39</v>
       </c>
-      <c r="AA13" s="10" t="n">
+      <c r="AA13" s="9" t="n">
         <v>117479570466.297</v>
       </c>
-      <c r="AB13" s="10" t="n">
+      <c r="AB13" s="9" t="n">
         <v>110332528947.917</v>
       </c>
-      <c r="AC13" s="10" t="n">
+      <c r="AC13" s="9" t="n">
         <v>114106065339.652</v>
       </c>
-      <c r="AD13" s="10" t="n">
+      <c r="AD13" s="9" t="n">
         <v>120511605998.347</v>
       </c>
-      <c r="AE13" s="10" t="n">
+      <c r="AE13" s="9" t="n">
         <v>120677406157.285</v>
       </c>
-      <c r="AF13" s="10" t="n">
+      <c r="AF13" s="9" t="n">
         <v>127331142588.759</v>
       </c>
-      <c r="AG13" s="10" t="n">
+      <c r="AG13" s="9" t="n">
         <v>125130764699.493</v>
       </c>
-      <c r="AH13" s="10" t="n">
+      <c r="AH13" s="9" t="n">
         <v>126548174525.055</v>
       </c>
-      <c r="AI13" s="10" t="n">
+      <c r="AI13" s="9" t="n">
         <v>123831747544.741</v>
       </c>
-      <c r="AJ13" s="10" t="n">
+      <c r="AJ13" s="9" t="n">
         <v>127278745636.945</v>
       </c>
-      <c r="AK13" s="10" t="n">
+      <c r="AK13" s="9" t="n">
         <v>136543637843.184</v>
       </c>
-      <c r="AL13" s="10"/>
-      <c r="AM13" s="10"/>
+      <c r="AL13" s="9"/>
+      <c r="AM13" s="9"/>
     </row>
     <row r="14">
       <c r="A14" t="str">
         <f>L14</f>
       </c>
-      <c r="B14" s="10" t="str">
+      <c r="B14" s="9" t="str">
         <f>AG14</f>
       </c>
-      <c r="C14" s="10" t="str">
+      <c r="C14" s="9" t="str">
         <f>AJ14</f>
       </c>
-      <c r="D14" s="10" t="str">
+      <c r="D14" s="9" t="str">
         <f>AK14</f>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="2" t="str">
         <f>AK14/AJ14-1</f>
       </c>
@@ -22854,98 +22854,98 @@
       <c r="L14" t="s">
         <v>55</v>
       </c>
-      <c r="M14" s="10" t="n">
+      <c r="M14" s="9" t="n">
         <v>110503273252.298</v>
       </c>
-      <c r="N14" s="10" t="n">
+      <c r="N14" s="9" t="n">
         <v>119914679039.574</v>
       </c>
-      <c r="O14" s="10" t="n">
+      <c r="O14" s="9" t="n">
         <v>141652862861.844</v>
       </c>
-      <c r="P14" s="10" t="n">
+      <c r="P14" s="9" t="n">
         <v>177949806499.254</v>
       </c>
-      <c r="Q14" s="10" t="n">
+      <c r="Q14" s="9" t="n">
         <v>176147389147.649</v>
       </c>
-      <c r="R14" s="10" t="n">
+      <c r="R14" s="9" t="n">
         <v>203179326295.875</v>
       </c>
-      <c r="S14" s="10" t="n">
+      <c r="S14" s="9" t="n">
         <v>220211529334.509</v>
       </c>
-      <c r="T14" s="10" t="n">
+      <c r="T14" s="9" t="n">
         <v>249612230141.979</v>
       </c>
-      <c r="U14" s="10" t="n">
+      <c r="U14" s="9" t="n">
         <v>279179355686.829</v>
       </c>
-      <c r="V14" s="10" t="n">
+      <c r="V14" s="9" t="n">
         <v>250237188317.358</v>
       </c>
-      <c r="W14" s="10" t="n">
+      <c r="W14" s="9" t="n">
         <v>279164675193.288</v>
       </c>
-      <c r="X14" s="10" t="n">
+      <c r="X14" s="9" t="n">
         <v>261597310509.72</v>
       </c>
-      <c r="Y14" s="10" t="n">
+      <c r="Y14" s="9" t="n">
         <v>250210300031.25</v>
       </c>
-      <c r="Z14" s="10" t="n">
+      <c r="Z14" s="9" t="n">
         <v>198943648804.73</v>
       </c>
-      <c r="AA14" s="10" t="n">
+      <c r="AA14" s="9" t="n">
         <v>189657877365.969</v>
       </c>
-      <c r="AB14" s="10" t="n">
+      <c r="AB14" s="9" t="n">
         <v>185391990129.497</v>
       </c>
-      <c r="AC14" s="10" t="n">
+      <c r="AC14" s="9" t="n">
         <v>201924898030.597</v>
       </c>
-      <c r="AD14" s="10" t="n">
+      <c r="AD14" s="9" t="n">
         <v>200712254029.102</v>
       </c>
-      <c r="AE14" s="10" t="n">
+      <c r="AE14" s="9" t="n">
         <v>222374993883.033</v>
       </c>
-      <c r="AF14" s="10" t="n">
+      <c r="AF14" s="9" t="n">
         <v>237875405256.288</v>
       </c>
-      <c r="AG14" s="10" t="n">
+      <c r="AG14" s="9" t="n">
         <v>258548030469.478</v>
       </c>
-      <c r="AH14" s="10" t="n">
+      <c r="AH14" s="9" t="n">
         <v>248243290872.247</v>
       </c>
-      <c r="AI14" s="10" t="n">
+      <c r="AI14" s="9" t="n">
         <v>239674836011.556</v>
       </c>
-      <c r="AJ14" s="10" t="n">
+      <c r="AJ14" s="9" t="n">
         <v>241088412575.15</v>
       </c>
-      <c r="AK14" s="10" t="n">
+      <c r="AK14" s="9" t="n">
         <v>235070426839.909</v>
       </c>
-      <c r="AL14" s="10"/>
-      <c r="AM14" s="10"/>
+      <c r="AL14" s="9"/>
+      <c r="AM14" s="9"/>
     </row>
     <row r="15">
       <c r="A15" t="str">
         <f>L15</f>
       </c>
-      <c r="B15" s="10" t="str">
+      <c r="B15" s="9" t="str">
         <f>AG15</f>
       </c>
-      <c r="C15" s="10" t="str">
+      <c r="C15" s="9" t="str">
         <f>AJ15</f>
       </c>
-      <c r="D15" s="10" t="str">
+      <c r="D15" s="9" t="str">
         <f>AK15</f>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="2" t="str">
         <f>AK15/AJ15-1</f>
       </c>
@@ -22960,98 +22960,98 @@
       <c r="L15" t="s">
         <v>56</v>
       </c>
-      <c r="M15" s="10" t="n">
+      <c r="M15" s="9" t="n">
         <v>10594679488.353</v>
       </c>
-      <c r="N15" s="10" t="n">
+      <c r="N15" s="9" t="n">
         <v>13944861852.608</v>
       </c>
-      <c r="O15" s="10" t="n">
+      <c r="O15" s="9" t="n">
         <v>13863626015.4369</v>
       </c>
-      <c r="P15" s="10" t="n">
+      <c r="P15" s="9" t="n">
         <v>16231728138.4242</v>
       </c>
-      <c r="Q15" s="10" t="n">
+      <c r="Q15" s="9" t="n">
         <v>17634555520.278</v>
       </c>
-      <c r="R15" s="10" t="n">
+      <c r="R15" s="9" t="n">
         <v>33227005483.805</v>
       </c>
-      <c r="S15" s="10" t="n">
+      <c r="S15" s="9" t="n">
         <v>28966730530.3942</v>
       </c>
-      <c r="T15" s="10" t="n">
+      <c r="T15" s="9" t="n">
         <v>24748527118.8072</v>
       </c>
-      <c r="U15" s="10" t="n">
+      <c r="U15" s="9" t="n">
         <v>32168507513.1468</v>
       </c>
-      <c r="V15" s="10" t="n">
+      <c r="V15" s="9" t="n">
         <v>34011351187.4841</v>
       </c>
-      <c r="W15" s="10" t="n">
+      <c r="W15" s="9" t="n">
         <v>23367402388.9989</v>
       </c>
-      <c r="X15" s="10" t="n">
+      <c r="X15" s="9" t="n">
         <v>26175603057.2243</v>
       </c>
-      <c r="Y15" s="10" t="n">
+      <c r="Y15" s="9" t="n">
         <v>35541256487.2553</v>
       </c>
-      <c r="Z15" s="10" t="n">
+      <c r="Z15" s="9" t="n">
         <v>23557886621.167</v>
       </c>
-      <c r="AA15" s="10" t="n">
+      <c r="AA15" s="9" t="n">
         <v>15002553870.1532</v>
       </c>
-      <c r="AB15" s="10" t="n">
+      <c r="AB15" s="9" t="n">
         <v>11243366844.9997</v>
       </c>
-      <c r="AC15" s="10" t="n">
+      <c r="AC15" s="9" t="n">
         <v>9162731235.234</v>
       </c>
-      <c r="AD15" s="10" t="n">
+      <c r="AD15" s="9" t="n">
         <v>11248330954.3122</v>
       </c>
-      <c r="AE15" s="10" t="n">
+      <c r="AE15" s="9" t="n">
         <v>12695304975.2372</v>
       </c>
-      <c r="AF15" s="10" t="n">
+      <c r="AF15" s="9" t="n">
         <v>11495677830.8937</v>
       </c>
-      <c r="AG15" s="10" t="n">
+      <c r="AG15" s="9" t="n">
         <v>10353071199.3225</v>
       </c>
-      <c r="AH15" s="10" t="n">
+      <c r="AH15" s="9" t="n">
         <v>11636787174.3834</v>
       </c>
-      <c r="AI15" s="10" t="n">
+      <c r="AI15" s="9" t="n">
         <v>18350285969.8313</v>
       </c>
-      <c r="AJ15" s="10" t="n">
+      <c r="AJ15" s="9" t="n">
         <v>16981868245.7354</v>
       </c>
-      <c r="AK15" s="10" t="n">
+      <c r="AK15" s="9" t="n">
         <v>17003105779.2759</v>
       </c>
-      <c r="AL15" s="10"/>
-      <c r="AM15" s="10"/>
+      <c r="AL15" s="9"/>
+      <c r="AM15" s="9"/>
     </row>
     <row r="16">
       <c r="A16" t="str">
         <f>L16</f>
       </c>
-      <c r="B16" s="10" t="str">
+      <c r="B16" s="9" t="str">
         <f>AG16</f>
       </c>
-      <c r="C16" s="10" t="str">
+      <c r="C16" s="9" t="str">
         <f>AJ16</f>
       </c>
-      <c r="D16" s="10" t="str">
+      <c r="D16" s="9" t="str">
         <f>AK16</f>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="2" t="str">
         <f>AK16/AJ16-1</f>
       </c>
@@ -23066,98 +23066,98 @@
       <c r="L16" t="s">
         <v>60</v>
       </c>
-      <c r="M16" s="10" t="n">
+      <c r="M16" s="9" t="n">
         <v>10310802233.5323</v>
       </c>
-      <c r="N16" s="10" t="n">
+      <c r="N16" s="9" t="n">
         <v>10164446007.0455</v>
       </c>
-      <c r="O16" s="10" t="n">
+      <c r="O16" s="9" t="n">
         <v>14594693221.8333</v>
       </c>
-      <c r="P16" s="10" t="n">
+      <c r="P16" s="9" t="n">
         <v>14395400805.4448</v>
       </c>
-      <c r="Q16" s="10" t="n">
+      <c r="Q16" s="9" t="n">
         <v>15210400882.0125</v>
       </c>
-      <c r="R16" s="10" t="n">
+      <c r="R16" s="9" t="n">
         <v>10279902836.0924</v>
       </c>
-      <c r="S16" s="10" t="n">
+      <c r="S16" s="9" t="n">
         <v>10302798298.1244</v>
       </c>
-      <c r="T16" s="10" t="n">
+      <c r="T16" s="9" t="n">
         <v>7859633339.78007</v>
       </c>
-      <c r="U16" s="10" t="n">
+      <c r="U16" s="9" t="n">
         <v>7420092697.17786</v>
       </c>
-      <c r="V16" s="10" t="n">
+      <c r="V16" s="9" t="n">
         <v>12778306414.2294</v>
       </c>
-      <c r="W16" s="10" t="n">
+      <c r="W16" s="9" t="n">
         <v>20330605753.9919</v>
       </c>
-      <c r="X16" s="10" t="n">
+      <c r="X16" s="9" t="n">
         <v>32721996106.4789</v>
       </c>
-      <c r="Y16" s="10" t="n">
+      <c r="Y16" s="9" t="n">
         <v>36463027220.7046</v>
       </c>
-      <c r="Z16" s="10" t="n">
+      <c r="Z16" s="9" t="n">
         <v>43954388258.5447</v>
       </c>
-      <c r="AA16" s="10" t="n">
+      <c r="AA16" s="9" t="n">
         <v>31695759762.263</v>
       </c>
-      <c r="AB16" s="10" t="n">
+      <c r="AB16" s="9" t="n">
         <v>32011684919.4972</v>
       </c>
-      <c r="AC16" s="10" t="n">
+      <c r="AC16" s="9" t="n">
         <v>41024920016.1634</v>
       </c>
-      <c r="AD16" s="10" t="n">
+      <c r="AD16" s="9" t="n">
         <v>55793420266.394</v>
       </c>
-      <c r="AE16" s="10" t="n">
+      <c r="AE16" s="9" t="n">
         <v>66713757130.9034</v>
       </c>
-      <c r="AF16" s="10" t="n">
+      <c r="AF16" s="9" t="n">
         <v>67556456875.3065</v>
       </c>
-      <c r="AG16" s="10" t="n">
+      <c r="AG16" s="9" t="n">
         <v>88895271810.8618</v>
       </c>
-      <c r="AH16" s="10" t="n">
+      <c r="AH16" s="9" t="n">
         <v>41749486569.6818</v>
       </c>
-      <c r="AI16" s="10" t="n">
+      <c r="AI16" s="9" t="n">
         <v>46523020544.609</v>
       </c>
-      <c r="AJ16" s="10" t="n">
+      <c r="AJ16" s="9" t="n">
         <v>64656951414.6669</v>
       </c>
-      <c r="AK16" s="10" t="n">
+      <c r="AK16" s="9" t="n">
         <v>37818450872.3933</v>
       </c>
-      <c r="AL16" s="10"/>
-      <c r="AM16" s="10"/>
+      <c r="AL16" s="9"/>
+      <c r="AM16" s="9"/>
     </row>
     <row r="17">
       <c r="A17" t="str">
         <f>L17</f>
       </c>
-      <c r="B17" s="10" t="str">
+      <c r="B17" s="9" t="str">
         <f>AG17</f>
       </c>
-      <c r="C17" s="10" t="str">
+      <c r="C17" s="9" t="str">
         <f>AJ17</f>
       </c>
-      <c r="D17" s="10" t="str">
+      <c r="D17" s="9" t="str">
         <f>AK17</f>
       </c>
-      <c r="E17" s="10"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="2" t="str">
         <f>AK17/AJ17-1</f>
       </c>
@@ -23170,98 +23170,98 @@
       </c>
       <c r="J17" s="2"/>
       <c r="L17"/>
-      <c r="M17" s="10" t="n">
+      <c r="M17" s="9" t="n">
         <v>11119152957.58</v>
       </c>
-      <c r="N17" s="10" t="n">
+      <c r="N17" s="9" t="n">
         <v>10544288449.1564</v>
       </c>
-      <c r="O17" s="10" t="n">
+      <c r="O17" s="9" t="n">
         <v>13707665483.978</v>
       </c>
-      <c r="P17" s="10" t="n">
+      <c r="P17" s="9" t="n">
         <v>14400719848.3348</v>
       </c>
-      <c r="Q17" s="10" t="n">
+      <c r="Q17" s="9" t="n">
         <v>14347823540.9574</v>
       </c>
-      <c r="R17" s="10" t="n">
+      <c r="R17" s="9" t="n">
         <v>11131070317.0259</v>
       </c>
-      <c r="S17" s="10" t="n">
+      <c r="S17" s="9" t="n">
         <v>6855489170.15793</v>
       </c>
-      <c r="T17" s="10" t="n">
+      <c r="T17" s="9" t="n">
         <v>1161233735.1637</v>
       </c>
-      <c r="U17" s="10" t="n">
+      <c r="U17" s="9" t="n">
         <v>8588612371.65704</v>
       </c>
-      <c r="V17" s="10" t="n">
+      <c r="V17" s="9" t="n">
         <v>4522801584.18371</v>
       </c>
-      <c r="W17" s="10" t="n">
+      <c r="W17" s="9" t="n">
         <v>291811804.184649</v>
       </c>
-      <c r="X17" s="10" t="n">
+      <c r="X17" s="9" t="n">
         <v>-4111788.83780017</v>
       </c>
-      <c r="Y17" s="10" t="n">
+      <c r="Y17" s="9" t="n">
         <v>-2585879.6769902</v>
       </c>
-      <c r="Z17" s="10" t="n">
+      <c r="Z17" s="9" t="n">
         <v>654852.128864949</v>
       </c>
-      <c r="AA17" s="10" t="n">
+      <c r="AA17" s="9" t="n">
         <v>-3583456.53012523</v>
       </c>
-      <c r="AB17" s="10" t="n">
+      <c r="AB17" s="9" t="n">
         <v>37531.3699317261</v>
       </c>
-      <c r="AC17" s="10" t="n">
+      <c r="AC17" s="9" t="n">
         <v>-72603.4972183619</v>
       </c>
-      <c r="AD17" s="10" t="n">
+      <c r="AD17" s="9" t="n">
         <v>1656165.43825815</v>
       </c>
-      <c r="AE17" s="10" t="n">
+      <c r="AE17" s="9" t="n">
         <v>24128.2435797438</v>
       </c>
-      <c r="AF17" s="10" t="n">
+      <c r="AF17" s="9" t="n">
         <v>59684.9236466806</v>
       </c>
-      <c r="AG17" s="10" t="n">
+      <c r="AG17" s="9" t="n">
         <v>11573.9072704938</v>
       </c>
-      <c r="AH17" s="10" t="n">
+      <c r="AH17" s="9" t="n">
         <v>11188.817598517</v>
       </c>
-      <c r="AI17" s="10" t="n">
+      <c r="AI17" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="AJ17" s="10" t="n">
+      <c r="AJ17" s="9" t="n">
         <v>-29324.9492</v>
       </c>
-      <c r="AK17" s="10" t="n">
+      <c r="AK17" s="9" t="n">
         <v>9739.88670259903</v>
       </c>
-      <c r="AL17" s="10"/>
-      <c r="AM17" s="10"/>
+      <c r="AL17" s="9"/>
+      <c r="AM17" s="9"/>
     </row>
     <row r="18">
       <c r="A18" t="str">
         <f>L18</f>
       </c>
-      <c r="B18" s="10" t="str">
+      <c r="B18" s="9" t="str">
         <f>AG18</f>
       </c>
-      <c r="C18" s="10" t="str">
+      <c r="C18" s="9" t="str">
         <f>AJ18</f>
       </c>
-      <c r="D18" s="10" t="str">
+      <c r="D18" s="9" t="str">
         <f>AK18</f>
       </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="2" t="str">
         <f>AK18/AJ18-1</f>
       </c>
@@ -23276,85 +23276,85 @@
       <c r="L18" t="s">
         <v>20</v>
       </c>
-      <c r="M18" s="10" t="str">
+      <c r="M18" s="9" t="str">
         <f>Sum(M12:M17)</f>
       </c>
-      <c r="N18" s="10" t="str">
+      <c r="N18" s="9" t="str">
         <f>Sum(N12:N17)</f>
       </c>
-      <c r="O18" s="10" t="str">
+      <c r="O18" s="9" t="str">
         <f>Sum(O12:O17)</f>
       </c>
-      <c r="P18" s="10" t="str">
+      <c r="P18" s="9" t="str">
         <f>Sum(P12:P17)</f>
       </c>
-      <c r="Q18" s="10" t="str">
+      <c r="Q18" s="9" t="str">
         <f>Sum(Q12:Q17)</f>
       </c>
-      <c r="R18" s="10" t="str">
+      <c r="R18" s="9" t="str">
         <f>Sum(R12:R17)</f>
       </c>
-      <c r="S18" s="10" t="str">
+      <c r="S18" s="9" t="str">
         <f>Sum(S12:S17)</f>
       </c>
-      <c r="T18" s="10" t="str">
+      <c r="T18" s="9" t="str">
         <f>Sum(T12:T17)</f>
       </c>
-      <c r="U18" s="10" t="str">
+      <c r="U18" s="9" t="str">
         <f>Sum(U12:U17)</f>
       </c>
-      <c r="V18" s="10" t="str">
+      <c r="V18" s="9" t="str">
         <f>Sum(V12:V17)</f>
       </c>
-      <c r="W18" s="10" t="str">
+      <c r="W18" s="9" t="str">
         <f>Sum(W12:W17)</f>
       </c>
-      <c r="X18" s="10" t="str">
+      <c r="X18" s="9" t="str">
         <f>Sum(X12:X17)</f>
       </c>
-      <c r="Y18" s="10" t="str">
+      <c r="Y18" s="9" t="str">
         <f>Sum(Y12:Y17)</f>
       </c>
-      <c r="Z18" s="10" t="str">
+      <c r="Z18" s="9" t="str">
         <f>Sum(Z12:Z17)</f>
       </c>
-      <c r="AA18" s="10" t="str">
+      <c r="AA18" s="9" t="str">
         <f>Sum(AA12:AA17)</f>
       </c>
-      <c r="AB18" s="10" t="str">
+      <c r="AB18" s="9" t="str">
         <f>Sum(AB12:AB17)</f>
       </c>
-      <c r="AC18" s="10" t="str">
+      <c r="AC18" s="9" t="str">
         <f>Sum(AC12:AC17)</f>
       </c>
-      <c r="AD18" s="10" t="str">
+      <c r="AD18" s="9" t="str">
         <f>Sum(AD12:AD17)</f>
       </c>
-      <c r="AE18" s="10" t="str">
+      <c r="AE18" s="9" t="str">
         <f>Sum(AE12:AE17)</f>
       </c>
-      <c r="AF18" s="10" t="str">
+      <c r="AF18" s="9" t="str">
         <f>Sum(AF12:AF17)</f>
       </c>
-      <c r="AG18" s="10" t="str">
+      <c r="AG18" s="9" t="str">
         <f>Sum(AG12:AG17)</f>
       </c>
-      <c r="AH18" s="10" t="str">
+      <c r="AH18" s="9" t="str">
         <f>Sum(AH12:AH17)</f>
       </c>
-      <c r="AI18" s="10" t="str">
+      <c r="AI18" s="9" t="str">
         <f>Sum(AI12:AI17)</f>
       </c>
-      <c r="AJ18" s="10" t="str">
+      <c r="AJ18" s="9" t="str">
         <f>Sum(AJ12:AJ17)</f>
       </c>
-      <c r="AK18" s="10" t="str">
+      <c r="AK18" s="9" t="str">
         <f>Sum(AK12:AK17)</f>
       </c>
-      <c r="AL18" s="10" t="str">
+      <c r="AL18" s="9" t="str">
         <f>Sum(AL12:AL17)</f>
       </c>
-      <c r="AM18" s="10"/>
+      <c r="AM18" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>